<commit_message>
Fixed graphs, changed chapter 5 index
</commit_message>
<xml_diff>
--- a/thesis-tests.xlsx
+++ b/thesis-tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguelanciaes/Desktop/thesis/novathesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D775239-CDFA-C24A-991B-F47D2FA4E2A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D469E4EF-FDB8-354E-A343-CCA741EE85B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{6308EBAC-DE62-D645-97F4-0D2E9D77B78B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{6308EBAC-DE62-D645-97F4-0D2E9D77B78B}"/>
   </bookViews>
   <sheets>
     <sheet name="External Redis-Benchmarks" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,6 @@
     <definedName name="tests_6" localSheetId="0">'External Redis-Benchmarks'!$C$40:$J$44</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -189,15 +188,6 @@
     <t>GET</t>
   </si>
   <si>
-    <t>Normal Redis</t>
-  </si>
-  <si>
-    <t>SGX Redis</t>
-  </si>
-  <si>
-    <t>Unsecure Redis</t>
-  </si>
-  <si>
     <t>Average</t>
   </si>
   <si>
@@ -208,6 +198,15 @@
   </si>
   <si>
     <t>Get</t>
+  </si>
+  <si>
+    <t>Vulnerable Redis</t>
+  </si>
+  <si>
+    <t>Built-in Secured Redis</t>
+  </si>
+  <si>
+    <t>SGX Secured Redis</t>
   </si>
 </sst>
 </file>
@@ -620,7 +619,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -638,16 +641,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,7 +748,15 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Normal Redis</c:v>
+            <c:strRef>
+              <c:f>'External Redis-Benchmarks'!$B$11:$J$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vulnerable Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -800,6 +807,7 @@
             </c:extLst>
           </c:dPt>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -814,7 +822,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -901,7 +909,15 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Unprotected Redis</c:v>
+            <c:strRef>
+              <c:f>'External Redis-Benchmarks'!$B$39:$J$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Built-in Secured Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -914,21 +930,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000019-A07C-8042-8AD6-CC030ED8774F}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -943,7 +945,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -959,11 +961,12 @@
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
+            <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -984,23 +987,6 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>('External Redis-Benchmarks'!$C$33,'External Redis-Benchmarks'!$C$35,'External Redis-Benchmarks'!$C$36)</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Ping</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Set</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Get</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>('External Redis-Benchmarks'!$E$61,'External Redis-Benchmarks'!$E$63,'External Redis-Benchmarks'!$E$64)</c:f>
@@ -1021,7 +1007,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000017-A07C-8042-8AD6-CC030ED8774F}"/>
+              <c16:uniqueId val="{00000009-FCDD-F44B-B413-4D6098EBFC3E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1029,7 +1015,15 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>SGX Redis</c:v>
+            <c:strRef>
+              <c:f>'External Redis-Benchmarks'!$B$66:$J$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SGX Secured Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -1042,6 +1036,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1056,7 +1051,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1180,7 +1175,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1223,7 +1218,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#\ ##0.000" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1600"/>
+                  <a:t>Milliseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#\ ##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1281,7 +1331,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1380,7 +1430,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Benchmark Throughput (op/s)</a:t>
+              <a:t> Benchmark Throughput</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -1426,7 +1476,15 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Normal Redis</c:v>
+            <c:strRef>
+              <c:f>'External Redis-Benchmarks'!$B$11:$J$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vulnerable Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -1439,6 +1497,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1453,7 +1512,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1540,7 +1599,15 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Unprotected Redis</c:v>
+            <c:strRef>
+              <c:f>'External Redis-Benchmarks'!$B$39:$J$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Built-in Secured Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -1553,6 +1620,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1567,7 +1635,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1654,7 +1722,15 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>SGX Redis</c:v>
+            <c:strRef>
+              <c:f>'External Redis-Benchmarks'!$B$66:$J$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SGX Secured Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -1667,6 +1743,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1681,7 +1758,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1799,7 +1876,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1842,7 +1919,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#\ ##0.000" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1600"/>
+                  <a:t>Operations</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1600" baseline="0"/>
+                  <a:t> Per Second</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#\ ##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1900,7 +2037,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2073,7 +2210,15 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Normal Redis</c:v>
+            <c:strRef>
+              <c:f>'Internal Redis-Benchmarks'!$B$11:$J$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vulnerable Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -2086,6 +2231,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.0000" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2100,7 +2246,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -2187,7 +2333,15 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Unprotected Redis</c:v>
+            <c:strRef>
+              <c:f>'Internal Redis-Benchmarks'!$B$39:$J$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Built-in Secured Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -2200,6 +2354,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.0000" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2214,7 +2369,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -2301,7 +2456,15 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>SGX Redis</c:v>
+            <c:strRef>
+              <c:f>'Internal Redis-Benchmarks'!$B$66:$J$66</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>SGX Secured Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -2314,6 +2477,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.0000" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2328,7 +2492,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -2453,7 +2617,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2496,7 +2660,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#\ ##0.000" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1600"/>
+                  <a:t>Milliseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#\ ##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2554,7 +2773,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2665,7 +2884,7 @@
               <a:rPr lang="en-GB" sz="1800" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Redis Benchmark Throughput (op/s)</a:t>
+              <a:t>Redis Benchmark Throughput</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB" sz="1400" b="0" i="0" baseline="0">
               <a:effectLst/>
@@ -2727,7 +2946,15 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Normal Redis</c:v>
+            <c:strRef>
+              <c:f>'Internal Redis-Benchmarks'!$B$11:$J$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vulnerable Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -2740,6 +2967,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2754,7 +2982,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -2841,7 +3069,15 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Unprotected Redis</c:v>
+            <c:strRef>
+              <c:f>'Internal Redis-Benchmarks'!$B$39:$J$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Built-in Secured Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -2854,6 +3090,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2868,7 +3105,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -2955,7 +3192,15 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>SGX Redis</c:v>
+            <c:strRef>
+              <c:f>'Internal Redis-Benchmarks'!$B$66:$J$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SGX Secured Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -2968,6 +3213,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2982,7 +3228,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -3107,7 +3353,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3150,7 +3396,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#\ ##0.000" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1600"/>
+                  <a:t>Operations Per Second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#\ ##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3208,7 +3509,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -5590,23 +5891,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_3" connectionId="2" xr16:uid="{493998F8-C237-CC45-95DE-DE52776EC4BA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_6" connectionId="6" xr16:uid="{F0609839-D860-594D-A6DC-121FFC03226C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_5" connectionId="4" xr16:uid="{F7C01357-A0B7-9C46-A14F-E3A5D11E2DD6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_1" connectionId="5" xr16:uid="{83893D2E-64E6-4141-91BF-17E4FBF6D821}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_2" connectionId="1" xr16:uid="{EE16474F-CCD2-364B-A607-51BAF623E71C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_3" connectionId="2" xr16:uid="{493998F8-C237-CC45-95DE-DE52776EC4BA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5908,8 +6209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF65E5F0-7FEC-2D44-A2C2-0F5F83647661}">
   <dimension ref="B2:J92"/>
   <sheetViews>
-    <sheetView topLeftCell="E23" zoomScale="75" workbookViewId="0">
-      <selection activeCell="M74" sqref="M74"/>
+    <sheetView tabSelected="1" topLeftCell="H26" zoomScale="92" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R68" sqref="R68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5967,17 +6268,17 @@
       <c r="B10" s="6"/>
     </row>
     <row r="11" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="33"/>
+      <c r="B11" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="37"/>
     </row>
     <row r="12" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
@@ -6009,7 +6310,7 @@
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="28">
+      <c r="B13" s="38">
         <v>1</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -6038,7 +6339,7 @@
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="29"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="9" t="s">
         <v>15</v>
       </c>
@@ -6065,7 +6366,7 @@
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="29"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="9" t="s">
         <v>16</v>
       </c>
@@ -6092,7 +6393,7 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="34"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="10" t="s">
         <v>17</v>
       </c>
@@ -6119,7 +6420,7 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="28">
+      <c r="B17" s="38">
         <v>2</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -6148,7 +6449,7 @@
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="29"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="9" t="s">
         <v>15</v>
       </c>
@@ -6175,7 +6476,7 @@
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="29"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="9" t="s">
         <v>16</v>
       </c>
@@ -6202,7 +6503,7 @@
       </c>
     </row>
     <row r="20" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="34"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="10" t="s">
         <v>17</v>
       </c>
@@ -6229,7 +6530,7 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="28">
+      <c r="B21" s="38">
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -6258,7 +6559,7 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="29"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="9" t="s">
         <v>15</v>
       </c>
@@ -6285,7 +6586,7 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="29"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="9" t="s">
         <v>16</v>
       </c>
@@ -6312,7 +6613,7 @@
       </c>
     </row>
     <row r="24" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="34"/>
+      <c r="B24" s="39"/>
       <c r="C24" s="10" t="s">
         <v>17</v>
       </c>
@@ -6339,7 +6640,7 @@
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="28">
+      <c r="B25" s="38">
         <v>4</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -6368,7 +6669,7 @@
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B26" s="29"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="9" t="s">
         <v>15</v>
       </c>
@@ -6395,7 +6696,7 @@
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="29"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="9" t="s">
         <v>16</v>
       </c>
@@ -6422,7 +6723,7 @@
       </c>
     </row>
     <row r="28" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="34"/>
+      <c r="B28" s="39"/>
       <c r="C28" s="10" t="s">
         <v>17</v>
       </c>
@@ -6449,7 +6750,7 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="28">
+      <c r="B29" s="38">
         <v>5</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -6478,7 +6779,7 @@
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B30" s="29"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="9" t="s">
         <v>15</v>
       </c>
@@ -6505,7 +6806,7 @@
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B31" s="29"/>
+      <c r="B31" s="33"/>
       <c r="C31" s="9" t="s">
         <v>16</v>
       </c>
@@ -6532,7 +6833,7 @@
       </c>
     </row>
     <row r="32" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="30"/>
+      <c r="B32" s="34"/>
       <c r="C32" s="14" t="s">
         <v>17</v>
       </c>
@@ -6559,11 +6860,11 @@
       </c>
     </row>
     <row r="33" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="35" t="s">
-        <v>21</v>
+      <c r="B33" s="32" t="s">
+        <v>18</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D33" s="25">
         <f>AVERAGE(D13,D17,D21,D25,D29)</f>
@@ -6595,7 +6896,7 @@
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="29"/>
+      <c r="B34" s="33"/>
       <c r="C34" s="9" t="s">
         <v>15</v>
       </c>
@@ -6629,9 +6930,9 @@
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B35" s="29"/>
+      <c r="B35" s="33"/>
       <c r="C35" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D35" s="19">
         <f>AVERAGE(D15,D19,D23,D27,D31)</f>
@@ -6663,9 +6964,9 @@
       </c>
     </row>
     <row r="36" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="30"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D36" s="23">
         <f>AVERAGE(D16,D20,D24,D28,D32)</f>
@@ -6699,17 +7000,17 @@
     <row r="37" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="33"/>
+      <c r="B39" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="36"/>
+      <c r="J39" s="37"/>
     </row>
     <row r="40" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="26" t="s">
@@ -6741,7 +7042,7 @@
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="28">
+      <c r="B41" s="38">
         <v>1</v>
       </c>
       <c r="C41" s="8" t="s">
@@ -6770,7 +7071,7 @@
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B42" s="29"/>
+      <c r="B42" s="33"/>
       <c r="C42" s="9" t="s">
         <v>15</v>
       </c>
@@ -6797,7 +7098,7 @@
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B43" s="29"/>
+      <c r="B43" s="33"/>
       <c r="C43" s="9" t="s">
         <v>16</v>
       </c>
@@ -6824,7 +7125,7 @@
       </c>
     </row>
     <row r="44" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="34"/>
+      <c r="B44" s="39"/>
       <c r="C44" s="10" t="s">
         <v>17</v>
       </c>
@@ -6851,7 +7152,7 @@
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B45" s="28">
+      <c r="B45" s="38">
         <v>2</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -6880,7 +7181,7 @@
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B46" s="29"/>
+      <c r="B46" s="33"/>
       <c r="C46" s="9" t="s">
         <v>15</v>
       </c>
@@ -6907,7 +7208,7 @@
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B47" s="29"/>
+      <c r="B47" s="33"/>
       <c r="C47" s="9" t="s">
         <v>16</v>
       </c>
@@ -6934,7 +7235,7 @@
       </c>
     </row>
     <row r="48" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="34"/>
+      <c r="B48" s="39"/>
       <c r="C48" s="10" t="s">
         <v>17</v>
       </c>
@@ -6961,7 +7262,7 @@
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B49" s="28">
+      <c r="B49" s="38">
         <v>3</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -6990,7 +7291,7 @@
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B50" s="29"/>
+      <c r="B50" s="33"/>
       <c r="C50" s="9" t="s">
         <v>15</v>
       </c>
@@ -7017,7 +7318,7 @@
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B51" s="29"/>
+      <c r="B51" s="33"/>
       <c r="C51" s="9" t="s">
         <v>16</v>
       </c>
@@ -7044,7 +7345,7 @@
       </c>
     </row>
     <row r="52" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="34"/>
+      <c r="B52" s="39"/>
       <c r="C52" s="10" t="s">
         <v>17</v>
       </c>
@@ -7071,7 +7372,7 @@
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B53" s="28">
+      <c r="B53" s="38">
         <v>4</v>
       </c>
       <c r="C53" s="8" t="s">
@@ -7100,7 +7401,7 @@
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B54" s="29"/>
+      <c r="B54" s="33"/>
       <c r="C54" s="9" t="s">
         <v>15</v>
       </c>
@@ -7127,7 +7428,7 @@
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B55" s="29"/>
+      <c r="B55" s="33"/>
       <c r="C55" s="9" t="s">
         <v>16</v>
       </c>
@@ -7154,7 +7455,7 @@
       </c>
     </row>
     <row r="56" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="34"/>
+      <c r="B56" s="39"/>
       <c r="C56" s="10" t="s">
         <v>17</v>
       </c>
@@ -7181,7 +7482,7 @@
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" s="28">
+      <c r="B57" s="38">
         <v>5</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -7210,7 +7511,7 @@
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B58" s="29"/>
+      <c r="B58" s="33"/>
       <c r="C58" s="9" t="s">
         <v>15</v>
       </c>
@@ -7237,7 +7538,7 @@
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B59" s="29"/>
+      <c r="B59" s="33"/>
       <c r="C59" s="9" t="s">
         <v>16</v>
       </c>
@@ -7264,7 +7565,7 @@
       </c>
     </row>
     <row r="60" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="30"/>
+      <c r="B60" s="34"/>
       <c r="C60" s="14" t="s">
         <v>17</v>
       </c>
@@ -7291,8 +7592,8 @@
       </c>
     </row>
     <row r="61" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="35" t="s">
-        <v>21</v>
+      <c r="B61" s="32" t="s">
+        <v>18</v>
       </c>
       <c r="C61" s="16" t="s">
         <v>14</v>
@@ -7327,7 +7628,7 @@
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B62" s="29"/>
+      <c r="B62" s="33"/>
       <c r="C62" s="9" t="s">
         <v>15</v>
       </c>
@@ -7361,7 +7662,7 @@
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B63" s="29"/>
+      <c r="B63" s="33"/>
       <c r="C63" s="9" t="s">
         <v>16</v>
       </c>
@@ -7395,7 +7696,7 @@
       </c>
     </row>
     <row r="64" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="30"/>
+      <c r="B64" s="34"/>
       <c r="C64" s="14" t="s">
         <v>17</v>
       </c>
@@ -7430,17 +7731,17 @@
     </row>
     <row r="65" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C66" s="32"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="32"/>
-      <c r="G66" s="32"/>
-      <c r="H66" s="32"/>
-      <c r="I66" s="32"/>
-      <c r="J66" s="33"/>
+      <c r="B66" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C66" s="36"/>
+      <c r="D66" s="36"/>
+      <c r="E66" s="36"/>
+      <c r="F66" s="36"/>
+      <c r="G66" s="36"/>
+      <c r="H66" s="36"/>
+      <c r="I66" s="36"/>
+      <c r="J66" s="37"/>
     </row>
     <row r="67" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B67" s="26" t="s">
@@ -7472,7 +7773,7 @@
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B68" s="28">
+      <c r="B68" s="38">
         <v>1</v>
       </c>
       <c r="C68" s="8" t="s">
@@ -7501,7 +7802,7 @@
       </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B69" s="29"/>
+      <c r="B69" s="33"/>
       <c r="C69" s="9" t="s">
         <v>15</v>
       </c>
@@ -7528,7 +7829,7 @@
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B70" s="29"/>
+      <c r="B70" s="33"/>
       <c r="C70" s="9" t="s">
         <v>16</v>
       </c>
@@ -7555,7 +7856,7 @@
       </c>
     </row>
     <row r="71" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="34"/>
+      <c r="B71" s="39"/>
       <c r="C71" s="10" t="s">
         <v>17</v>
       </c>
@@ -7582,7 +7883,7 @@
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B72" s="28">
+      <c r="B72" s="38">
         <v>2</v>
       </c>
       <c r="C72" s="8" t="s">
@@ -7611,7 +7912,7 @@
       </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B73" s="29"/>
+      <c r="B73" s="33"/>
       <c r="C73" s="9" t="s">
         <v>15</v>
       </c>
@@ -7638,7 +7939,7 @@
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B74" s="29"/>
+      <c r="B74" s="33"/>
       <c r="C74" s="9" t="s">
         <v>16</v>
       </c>
@@ -7665,7 +7966,7 @@
       </c>
     </row>
     <row r="75" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="34"/>
+      <c r="B75" s="39"/>
       <c r="C75" s="10" t="s">
         <v>17</v>
       </c>
@@ -7692,7 +7993,7 @@
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B76" s="28">
+      <c r="B76" s="38">
         <v>3</v>
       </c>
       <c r="C76" s="8" t="s">
@@ -7721,7 +8022,7 @@
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B77" s="29"/>
+      <c r="B77" s="33"/>
       <c r="C77" s="9" t="s">
         <v>15</v>
       </c>
@@ -7748,7 +8049,7 @@
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B78" s="29"/>
+      <c r="B78" s="33"/>
       <c r="C78" s="9" t="s">
         <v>16</v>
       </c>
@@ -7775,7 +8076,7 @@
       </c>
     </row>
     <row r="79" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="34"/>
+      <c r="B79" s="39"/>
       <c r="C79" s="10" t="s">
         <v>17</v>
       </c>
@@ -7802,7 +8103,7 @@
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B80" s="28">
+      <c r="B80" s="38">
         <v>4</v>
       </c>
       <c r="C80" s="8" t="s">
@@ -7831,7 +8132,7 @@
       </c>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B81" s="29"/>
+      <c r="B81" s="33"/>
       <c r="C81" s="9" t="s">
         <v>15</v>
       </c>
@@ -7858,7 +8159,7 @@
       </c>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B82" s="29"/>
+      <c r="B82" s="33"/>
       <c r="C82" s="9" t="s">
         <v>16</v>
       </c>
@@ -7885,7 +8186,7 @@
       </c>
     </row>
     <row r="83" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="34"/>
+      <c r="B83" s="39"/>
       <c r="C83" s="10" t="s">
         <v>17</v>
       </c>
@@ -7912,7 +8213,7 @@
       </c>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B84" s="28">
+      <c r="B84" s="38">
         <v>5</v>
       </c>
       <c r="C84" s="8" t="s">
@@ -7941,7 +8242,7 @@
       </c>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B85" s="29"/>
+      <c r="B85" s="33"/>
       <c r="C85" s="9" t="s">
         <v>15</v>
       </c>
@@ -7968,7 +8269,7 @@
       </c>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B86" s="29"/>
+      <c r="B86" s="33"/>
       <c r="C86" s="9" t="s">
         <v>16</v>
       </c>
@@ -7995,7 +8296,7 @@
       </c>
     </row>
     <row r="87" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="30"/>
+      <c r="B87" s="34"/>
       <c r="C87" s="14" t="s">
         <v>17</v>
       </c>
@@ -8022,8 +8323,8 @@
       </c>
     </row>
     <row r="88" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="35" t="s">
-        <v>21</v>
+      <c r="B88" s="32" t="s">
+        <v>18</v>
       </c>
       <c r="C88" s="16" t="s">
         <v>14</v>
@@ -8058,7 +8359,7 @@
       </c>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B89" s="29"/>
+      <c r="B89" s="33"/>
       <c r="C89" s="9" t="s">
         <v>15</v>
       </c>
@@ -8092,7 +8393,7 @@
       </c>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B90" s="29"/>
+      <c r="B90" s="33"/>
       <c r="C90" s="9" t="s">
         <v>16</v>
       </c>
@@ -8126,7 +8427,7 @@
       </c>
     </row>
     <row r="91" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="30"/>
+      <c r="B91" s="34"/>
       <c r="C91" s="14" t="s">
         <v>17</v>
       </c>
@@ -8162,6 +8463,12 @@
     <row r="92" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B25:B28"/>
     <mergeCell ref="B61:B64"/>
     <mergeCell ref="B33:B36"/>
     <mergeCell ref="B88:B91"/>
@@ -8177,12 +8484,6 @@
     <mergeCell ref="B49:B52"/>
     <mergeCell ref="B53:B56"/>
     <mergeCell ref="B57:B60"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="B11:J11"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B25:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8193,8 +8494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1D7AB5-56EB-A14B-8A61-C582BDE41FCF}">
   <dimension ref="B2:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="75" workbookViewId="0">
-      <selection activeCell="P68" sqref="P68"/>
+    <sheetView topLeftCell="J34" zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8252,17 +8553,17 @@
       <c r="B10" s="6"/>
     </row>
     <row r="11" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="33"/>
+      <c r="B11" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="37"/>
     </row>
     <row r="12" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
@@ -8294,7 +8595,7 @@
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="28">
+      <c r="B13" s="38">
         <v>1</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -8323,7 +8624,7 @@
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="29"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="9" t="s">
         <v>15</v>
       </c>
@@ -8350,7 +8651,7 @@
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="29"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="9" t="s">
         <v>16</v>
       </c>
@@ -8377,7 +8678,7 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="34"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="10" t="s">
         <v>17</v>
       </c>
@@ -8404,7 +8705,7 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="28">
+      <c r="B17" s="38">
         <v>2</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -8433,7 +8734,7 @@
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="29"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="9" t="s">
         <v>15</v>
       </c>
@@ -8460,7 +8761,7 @@
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="29"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="9" t="s">
         <v>16</v>
       </c>
@@ -8487,7 +8788,7 @@
       </c>
     </row>
     <row r="20" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="34"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="10" t="s">
         <v>17</v>
       </c>
@@ -8514,7 +8815,7 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="28">
+      <c r="B21" s="38">
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -8543,7 +8844,7 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="29"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="9" t="s">
         <v>15</v>
       </c>
@@ -8570,7 +8871,7 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="29"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="9" t="s">
         <v>16</v>
       </c>
@@ -8597,7 +8898,7 @@
       </c>
     </row>
     <row r="24" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="34"/>
+      <c r="B24" s="39"/>
       <c r="C24" s="10" t="s">
         <v>17</v>
       </c>
@@ -8624,7 +8925,7 @@
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="28">
+      <c r="B25" s="38">
         <v>4</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -8653,7 +8954,7 @@
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B26" s="29"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="9" t="s">
         <v>15</v>
       </c>
@@ -8680,7 +8981,7 @@
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="29"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="9" t="s">
         <v>16</v>
       </c>
@@ -8707,7 +9008,7 @@
       </c>
     </row>
     <row r="28" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="34"/>
+      <c r="B28" s="39"/>
       <c r="C28" s="10" t="s">
         <v>17</v>
       </c>
@@ -8734,7 +9035,7 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="28">
+      <c r="B29" s="38">
         <v>5</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -8763,7 +9064,7 @@
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B30" s="29"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="9" t="s">
         <v>15</v>
       </c>
@@ -8790,7 +9091,7 @@
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B31" s="29"/>
+      <c r="B31" s="33"/>
       <c r="C31" s="9" t="s">
         <v>16</v>
       </c>
@@ -8817,7 +9118,7 @@
       </c>
     </row>
     <row r="32" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="30"/>
+      <c r="B32" s="34"/>
       <c r="C32" s="14" t="s">
         <v>17</v>
       </c>
@@ -8844,13 +9145,13 @@
       </c>
     </row>
     <row r="33" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="35" t="s">
-        <v>21</v>
+      <c r="B33" s="32" t="s">
+        <v>18</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="37">
+        <v>19</v>
+      </c>
+      <c r="D33" s="29">
         <f>AVERAGE(D13,D17,D21,D25,D29)</f>
         <v>159477.614</v>
       </c>
@@ -8874,17 +9175,17 @@
         <f t="shared" si="0"/>
         <v>0.3014</v>
       </c>
-      <c r="J33" s="36">
+      <c r="J33" s="28">
         <f t="shared" si="0"/>
         <v>0.85179999999999989</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="29"/>
+      <c r="B34" s="33"/>
       <c r="C34" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="38">
+      <c r="D34" s="30">
         <f t="shared" ref="D34:J34" si="1">AVERAGE(D14,D18,D22,D26,D30)</f>
         <v>157095.106</v>
       </c>
@@ -8914,11 +9215,11 @@
       </c>
     </row>
     <row r="35" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="29"/>
+      <c r="B35" s="33"/>
       <c r="C35" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" s="38">
+        <v>20</v>
+      </c>
+      <c r="D35" s="30">
         <f t="shared" ref="D35:J35" si="2">AVERAGE(D15,D19,D23,D27,D31)</f>
         <v>154979.29199999999</v>
       </c>
@@ -8948,11 +9249,11 @@
       </c>
     </row>
     <row r="36" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="30"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="39">
+        <v>21</v>
+      </c>
+      <c r="D36" s="31">
         <f t="shared" ref="D36:J36" si="3">AVERAGE(D16,D20,D24,D28,D32)</f>
         <v>157071.03400000001</v>
       </c>
@@ -8984,17 +9285,17 @@
     <row r="37" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="33"/>
+      <c r="B39" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="36"/>
+      <c r="J39" s="37"/>
     </row>
     <row r="40" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="26" t="s">
@@ -9026,7 +9327,7 @@
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="28">
+      <c r="B41" s="38">
         <v>1</v>
       </c>
       <c r="C41" s="8" t="s">
@@ -9055,7 +9356,7 @@
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B42" s="29"/>
+      <c r="B42" s="33"/>
       <c r="C42" s="9" t="s">
         <v>15</v>
       </c>
@@ -9082,7 +9383,7 @@
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B43" s="29"/>
+      <c r="B43" s="33"/>
       <c r="C43" s="9" t="s">
         <v>16</v>
       </c>
@@ -9109,7 +9410,7 @@
       </c>
     </row>
     <row r="44" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="34"/>
+      <c r="B44" s="39"/>
       <c r="C44" s="10" t="s">
         <v>17</v>
       </c>
@@ -9136,7 +9437,7 @@
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B45" s="28">
+      <c r="B45" s="38">
         <v>2</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -9165,7 +9466,7 @@
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B46" s="29"/>
+      <c r="B46" s="33"/>
       <c r="C46" s="9" t="s">
         <v>15</v>
       </c>
@@ -9192,7 +9493,7 @@
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B47" s="29"/>
+      <c r="B47" s="33"/>
       <c r="C47" s="9" t="s">
         <v>16</v>
       </c>
@@ -9219,7 +9520,7 @@
       </c>
     </row>
     <row r="48" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="34"/>
+      <c r="B48" s="39"/>
       <c r="C48" s="10" t="s">
         <v>17</v>
       </c>
@@ -9246,7 +9547,7 @@
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B49" s="28">
+      <c r="B49" s="38">
         <v>3</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -9275,7 +9576,7 @@
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B50" s="29"/>
+      <c r="B50" s="33"/>
       <c r="C50" s="9" t="s">
         <v>15</v>
       </c>
@@ -9302,7 +9603,7 @@
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B51" s="29"/>
+      <c r="B51" s="33"/>
       <c r="C51" s="9" t="s">
         <v>16</v>
       </c>
@@ -9329,7 +9630,7 @@
       </c>
     </row>
     <row r="52" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="34"/>
+      <c r="B52" s="39"/>
       <c r="C52" s="10" t="s">
         <v>17</v>
       </c>
@@ -9356,7 +9657,7 @@
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B53" s="28">
+      <c r="B53" s="38">
         <v>4</v>
       </c>
       <c r="C53" s="8" t="s">
@@ -9385,7 +9686,7 @@
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B54" s="29"/>
+      <c r="B54" s="33"/>
       <c r="C54" s="9" t="s">
         <v>15</v>
       </c>
@@ -9412,7 +9713,7 @@
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B55" s="29"/>
+      <c r="B55" s="33"/>
       <c r="C55" s="9" t="s">
         <v>16</v>
       </c>
@@ -9439,7 +9740,7 @@
       </c>
     </row>
     <row r="56" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="34"/>
+      <c r="B56" s="39"/>
       <c r="C56" s="10" t="s">
         <v>17</v>
       </c>
@@ -9466,7 +9767,7 @@
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" s="28">
+      <c r="B57" s="38">
         <v>5</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -9495,7 +9796,7 @@
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B58" s="29"/>
+      <c r="B58" s="33"/>
       <c r="C58" s="9" t="s">
         <v>15</v>
       </c>
@@ -9522,7 +9823,7 @@
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B59" s="29"/>
+      <c r="B59" s="33"/>
       <c r="C59" s="9" t="s">
         <v>16</v>
       </c>
@@ -9549,7 +9850,7 @@
       </c>
     </row>
     <row r="60" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="30"/>
+      <c r="B60" s="34"/>
       <c r="C60" s="14" t="s">
         <v>17</v>
       </c>
@@ -9576,8 +9877,8 @@
       </c>
     </row>
     <row r="61" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="35" t="s">
-        <v>21</v>
+      <c r="B61" s="32" t="s">
+        <v>18</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>14</v>
@@ -9606,13 +9907,13 @@
         <f t="shared" si="4"/>
         <v>0.2646</v>
       </c>
-      <c r="J61" s="36">
+      <c r="J61" s="28">
         <f t="shared" si="4"/>
         <v>35.058199999999999</v>
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B62" s="29"/>
+      <c r="B62" s="33"/>
       <c r="C62" s="9" t="s">
         <v>15</v>
       </c>
@@ -9646,7 +9947,7 @@
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B63" s="29"/>
+      <c r="B63" s="33"/>
       <c r="C63" s="9" t="s">
         <v>16</v>
       </c>
@@ -9680,7 +9981,7 @@
       </c>
     </row>
     <row r="64" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="30"/>
+      <c r="B64" s="34"/>
       <c r="C64" s="14" t="s">
         <v>17</v>
       </c>
@@ -9715,17 +10016,17 @@
     </row>
     <row r="65" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C66" s="32"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="32"/>
-      <c r="G66" s="32"/>
-      <c r="H66" s="32"/>
-      <c r="I66" s="32"/>
-      <c r="J66" s="33"/>
+      <c r="B66" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C66" s="36"/>
+      <c r="D66" s="36"/>
+      <c r="E66" s="36"/>
+      <c r="F66" s="36"/>
+      <c r="G66" s="36"/>
+      <c r="H66" s="36"/>
+      <c r="I66" s="36"/>
+      <c r="J66" s="37"/>
     </row>
     <row r="67" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B67" s="26" t="s">
@@ -9757,7 +10058,7 @@
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B68" s="28">
+      <c r="B68" s="38">
         <v>1</v>
       </c>
       <c r="C68" s="8" t="s">
@@ -9786,7 +10087,7 @@
       </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B69" s="29"/>
+      <c r="B69" s="33"/>
       <c r="C69" s="9" t="s">
         <v>15</v>
       </c>
@@ -9813,7 +10114,7 @@
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B70" s="29"/>
+      <c r="B70" s="33"/>
       <c r="C70" s="9" t="s">
         <v>16</v>
       </c>
@@ -9840,7 +10141,7 @@
       </c>
     </row>
     <row r="71" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="34"/>
+      <c r="B71" s="39"/>
       <c r="C71" s="10" t="s">
         <v>17</v>
       </c>
@@ -9867,7 +10168,7 @@
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B72" s="28">
+      <c r="B72" s="38">
         <v>2</v>
       </c>
       <c r="C72" s="8" t="s">
@@ -9896,7 +10197,7 @@
       </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B73" s="29"/>
+      <c r="B73" s="33"/>
       <c r="C73" s="9" t="s">
         <v>15</v>
       </c>
@@ -9923,7 +10224,7 @@
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B74" s="29"/>
+      <c r="B74" s="33"/>
       <c r="C74" s="9" t="s">
         <v>16</v>
       </c>
@@ -9950,7 +10251,7 @@
       </c>
     </row>
     <row r="75" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="34"/>
+      <c r="B75" s="39"/>
       <c r="C75" s="10" t="s">
         <v>17</v>
       </c>
@@ -9977,7 +10278,7 @@
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B76" s="28">
+      <c r="B76" s="38">
         <v>3</v>
       </c>
       <c r="C76" s="8" t="s">
@@ -10006,7 +10307,7 @@
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B77" s="29"/>
+      <c r="B77" s="33"/>
       <c r="C77" s="9" t="s">
         <v>15</v>
       </c>
@@ -10033,7 +10334,7 @@
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B78" s="29"/>
+      <c r="B78" s="33"/>
       <c r="C78" s="9" t="s">
         <v>16</v>
       </c>
@@ -10060,7 +10361,7 @@
       </c>
     </row>
     <row r="79" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="34"/>
+      <c r="B79" s="39"/>
       <c r="C79" s="10" t="s">
         <v>17</v>
       </c>
@@ -10087,7 +10388,7 @@
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B80" s="28">
+      <c r="B80" s="38">
         <v>4</v>
       </c>
       <c r="C80" s="8" t="s">
@@ -10116,7 +10417,7 @@
       </c>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B81" s="29"/>
+      <c r="B81" s="33"/>
       <c r="C81" s="9" t="s">
         <v>15</v>
       </c>
@@ -10143,7 +10444,7 @@
       </c>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B82" s="29"/>
+      <c r="B82" s="33"/>
       <c r="C82" s="9" t="s">
         <v>16</v>
       </c>
@@ -10170,7 +10471,7 @@
       </c>
     </row>
     <row r="83" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="34"/>
+      <c r="B83" s="39"/>
       <c r="C83" s="10" t="s">
         <v>17</v>
       </c>
@@ -10197,7 +10498,7 @@
       </c>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B84" s="28">
+      <c r="B84" s="38">
         <v>5</v>
       </c>
       <c r="C84" s="8" t="s">
@@ -10226,7 +10527,7 @@
       </c>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B85" s="29"/>
+      <c r="B85" s="33"/>
       <c r="C85" s="9" t="s">
         <v>15</v>
       </c>
@@ -10253,7 +10554,7 @@
       </c>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B86" s="29"/>
+      <c r="B86" s="33"/>
       <c r="C86" s="9" t="s">
         <v>16</v>
       </c>
@@ -10280,7 +10581,7 @@
       </c>
     </row>
     <row r="87" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="30"/>
+      <c r="B87" s="34"/>
       <c r="C87" s="14" t="s">
         <v>17</v>
       </c>
@@ -10307,8 +10608,8 @@
       </c>
     </row>
     <row r="88" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="35" t="s">
-        <v>21</v>
+      <c r="B88" s="32" t="s">
+        <v>18</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>14</v>
@@ -10337,13 +10638,13 @@
         <f t="shared" si="8"/>
         <v>4.4118000000000013</v>
       </c>
-      <c r="J88" s="36">
+      <c r="J88" s="28">
         <f t="shared" si="8"/>
         <v>124.38939999999998</v>
       </c>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B89" s="29"/>
+      <c r="B89" s="33"/>
       <c r="C89" s="9" t="s">
         <v>15</v>
       </c>
@@ -10377,7 +10678,7 @@
       </c>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B90" s="29"/>
+      <c r="B90" s="33"/>
       <c r="C90" s="9" t="s">
         <v>16</v>
       </c>
@@ -10411,7 +10712,7 @@
       </c>
     </row>
     <row r="91" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="30"/>
+      <c r="B91" s="34"/>
       <c r="C91" s="14" t="s">
         <v>17</v>
       </c>
@@ -10447,6 +10748,18 @@
     <row r="92" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="B39:J39"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="B49:B52"/>
     <mergeCell ref="B80:B83"/>
     <mergeCell ref="B84:B87"/>
     <mergeCell ref="B88:B91"/>
@@ -10456,18 +10769,6 @@
     <mergeCell ref="B68:B71"/>
     <mergeCell ref="B72:B75"/>
     <mergeCell ref="B76:B79"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="B39:J39"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="B11:J11"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B29:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added redis-benchmark graps to the report
</commit_message>
<xml_diff>
--- a/thesis-tests.xlsx
+++ b/thesis-tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguelanciaes/Desktop/thesis/novathesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D469E4EF-FDB8-354E-A343-CCA741EE85B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908B5F50-97DB-0540-9113-93CB6EB43372}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{6308EBAC-DE62-D645-97F4-0D2E9D77B78B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{6308EBAC-DE62-D645-97F4-0D2E9D77B78B}"/>
   </bookViews>
   <sheets>
     <sheet name="External Redis-Benchmarks" sheetId="2" r:id="rId1"/>
@@ -1497,7 +1497,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1512,7 +1512,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1620,7 +1620,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1635,7 +1635,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1743,7 +1743,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1758,7 +1758,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1926,7 +1926,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1939,14 +1939,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1600"/>
+                  <a:rPr lang="en-GB" sz="1200"/>
                   <a:t>Operations</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1600" baseline="0"/>
+                  <a:rPr lang="en-GB" sz="1200" baseline="0"/>
                   <a:t> Per Second</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-GB" sz="1600"/>
+                <a:endParaRPr lang="en-GB" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1963,7 +1963,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1995,7 +1995,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2098,6 +2098,712 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Redis</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Benchmark Latency</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'External Redis-Benchmarks'!$B$11:$J$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vulnerable Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>('External Redis-Benchmarks'!$C$33,'External Redis-Benchmarks'!$C$35,'External Redis-Benchmarks'!$C$36)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Ping</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Set</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Get</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('External Redis-Benchmarks'!$E$33,'External Redis-Benchmarks'!$E$35,'External Redis-Benchmarks'!$E$36)</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>39.444800000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.435199999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39.427000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B60A-F945-B358-0D6F141B9E50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'External Redis-Benchmarks'!$B$39:$J$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Built-in Secured Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>('External Redis-Benchmarks'!$C$33,'External Redis-Benchmarks'!$C$35,'External Redis-Benchmarks'!$C$36)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Ping</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Set</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Get</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('External Redis-Benchmarks'!$E$61,'External Redis-Benchmarks'!$E$63,'External Redis-Benchmarks'!$E$64)</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>39.8262</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.905799999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39.865400000000008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B60A-F945-B358-0D6F141B9E50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'External Redis-Benchmarks'!$B$66:$J$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SGX Secured Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>('External Redis-Benchmarks'!$C$33,'External Redis-Benchmarks'!$C$35,'External Redis-Benchmarks'!$C$36)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Ping</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Set</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Get</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('External Redis-Benchmarks'!$E$88,'External Redis-Benchmarks'!$E$90,'External Redis-Benchmarks'!$E$91)</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>41.738999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41.863599999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.827199999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B60A-F945-B358-0D6F141B9E50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1947686256"/>
+        <c:axId val="209290559"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1947686256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="209290559"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="209290559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:t>Operations</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+                  <a:t> Per Second</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1947686256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -2833,7 +3539,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -3569,6 +4275,1548 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Redis</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Benchmark Latency</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Internal Redis-Benchmarks'!$B$11:$J$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vulnerable Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>('Internal Redis-Benchmarks'!$C$33,'Internal Redis-Benchmarks'!$C$35,'Internal Redis-Benchmarks'!$C$36)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Ping</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Set</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Get</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Internal Redis-Benchmarks'!$E$33,'Internal Redis-Benchmarks'!$E$35,'Internal Redis-Benchmarks'!$E$36)</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.18099999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18339999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18119999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F9CB-3C42-99EE-C3682364CEB9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Internal Redis-Benchmarks'!$B$39:$J$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Built-in Secured Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>('Internal Redis-Benchmarks'!$C$33,'Internal Redis-Benchmarks'!$C$35,'Internal Redis-Benchmarks'!$C$36)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Ping</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Set</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Get</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Internal Redis-Benchmarks'!$E$61,'Internal Redis-Benchmarks'!$E$63,'Internal Redis-Benchmarks'!$E$64)</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.19839999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.20539999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2056</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F9CB-3C42-99EE-C3682364CEB9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Internal Redis-Benchmarks'!$B$66:$J$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SGX Secured Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>('Internal Redis-Benchmarks'!$C$33,'Internal Redis-Benchmarks'!$C$35,'Internal Redis-Benchmarks'!$C$36)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Ping</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Set</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Get</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Internal Redis-Benchmarks'!$E$88,'Internal Redis-Benchmarks'!$E$90,'Internal Redis-Benchmarks'!$E$91)</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.8329999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7796000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7822000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F9CB-3C42-99EE-C3682364CEB9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1947686256"/>
+        <c:axId val="209290559"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1947686256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="209290559"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="209290559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:t>Operations</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+                  <a:t> Per Second</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1947686256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Redis</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Benchmark Throughput</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Internal Redis-Benchmarks'!$B$11:$J$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vulnerable Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>('Internal Redis-Benchmarks'!$C$33,'Internal Redis-Benchmarks'!$C$35,'Internal Redis-Benchmarks'!$C$36)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Ping</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Set</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Get</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Internal Redis-Benchmarks'!$D$33,'Internal Redis-Benchmarks'!$D$35,'Internal Redis-Benchmarks'!$D$36)</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>159477.614</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>154979.29199999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>157071.03400000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-76AB-D742-9205-2EC3B4F80AA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Internal Redis-Benchmarks'!$B$39:$J$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Built-in Secured Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.3972982358422094E-2"/>
+                  <c:y val="7.8282253135836047E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-76AB-D742-9205-2EC3B4F80AA1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.7466227948027595E-2"/>
+                  <c:y val="3.9141126567918023E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-76AB-D742-9205-2EC3B4F80AA1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.9212850742830294E-2"/>
+                  <c:y val="3.9141126567918379E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-76AB-D742-9205-2EC3B4F80AA1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>('Internal Redis-Benchmarks'!$C$33,'Internal Redis-Benchmarks'!$C$35,'Internal Redis-Benchmarks'!$C$36)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Ping</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Set</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Get</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Internal Redis-Benchmarks'!$D$61,'Internal Redis-Benchmarks'!$D$63,'Internal Redis-Benchmarks'!$D$64)</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>133159.57999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128920.31000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>126850.876</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-76AB-D742-9205-2EC3B4F80AA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Internal Redis-Benchmarks'!$B$66:$J$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SGX Secured Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.2226359563619392E-2"/>
+                  <c:y val="3.9141126567916584E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-76AB-D742-9205-2EC3B4F80AA1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.5719605153224955E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-76AB-D742-9205-2EC3B4F80AA1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.3972982358422125E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-76AB-D742-9205-2EC3B4F80AA1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-PT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>('Internal Redis-Benchmarks'!$C$33,'Internal Redis-Benchmarks'!$C$35,'Internal Redis-Benchmarks'!$C$36)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Ping</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Set</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Get</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Internal Redis-Benchmarks'!$D$88,'Internal Redis-Benchmarks'!$D$90,'Internal Redis-Benchmarks'!$D$91)</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>17363.324000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17670.458000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17681.723999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-76AB-D742-9205-2EC3B4F80AA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1947686256"/>
+        <c:axId val="209290559"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1947686256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="209290559"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="209290559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:t>Operations</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+                  <a:t> Per Second</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#\ ##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1947686256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3729,6 +5977,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4727,7 +7095,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4750,17 +7118,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
@@ -4931,22 +7288,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -5051,8 +7409,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5184,19 +7542,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -5700,6 +8059,1497 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -5773,15 +9623,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
+      <xdr:colOff>594753</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>31749</xdr:rowOff>
+      <xdr:rowOff>28231</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>265165</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>83736</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>560888</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>19160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5801,6 +9651,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>589561</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>101607</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>555696</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>1096</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FC9B916-BB90-0F46-BC0F-B8D1AFB99AC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5878,6 +9766,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>667175</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>82369</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C81C5CE-1DA2-344D-B085-DAADBDDEE102}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>667175</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>133169</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74CE4C78-55BF-FD4B-A6F4-B2306B77D93C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6209,8 +10173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF65E5F0-7FEC-2D44-A2C2-0F5F83647661}">
   <dimension ref="B2:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H26" zoomScale="92" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R68" sqref="R68"/>
+    <sheetView topLeftCell="A12" zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="U56" sqref="U56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8494,8 +12458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1D7AB5-56EB-A14B-8A61-C582BDE41FCF}">
   <dimension ref="B2:J92"/>
   <sheetViews>
-    <sheetView topLeftCell="J34" zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="R26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC32" sqref="AC32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Written chapter 5 introduction, 5.1, 5.2 and first testbench - 5.3
</commit_message>
<xml_diff>
--- a/thesis-tests.xlsx
+++ b/thesis-tests.xlsx
@@ -8,15 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguelanciaes/Desktop/thesis/novathesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908B5F50-97DB-0540-9113-93CB6EB43372}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2A5037-7E01-1A4C-BB98-8AFAC46AE352}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{6308EBAC-DE62-D645-97F4-0D2E9D77B78B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{6308EBAC-DE62-D645-97F4-0D2E9D77B78B}"/>
   </bookViews>
   <sheets>
     <sheet name="External Redis-Benchmarks" sheetId="2" r:id="rId1"/>
     <sheet name="Internal Redis-Benchmarks" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'External Redis-Benchmarks'!$B$11:$J$11</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'External Redis-Benchmarks'!$B$39:$J$39</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'External Redis-Benchmarks'!$B$66:$J$66</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">('External Redis-Benchmarks'!$C$33,'External Redis-Benchmarks'!$C$35,'External Redis-Benchmarks'!$C$36)</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">('External Redis-Benchmarks'!$E$33,'External Redis-Benchmarks'!$E$35,'External Redis-Benchmarks'!$E$36)</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">('External Redis-Benchmarks'!$E$61,'External Redis-Benchmarks'!$E$63,'External Redis-Benchmarks'!$E$64)</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">('External Redis-Benchmarks'!$E$88,'External Redis-Benchmarks'!$E$90,'External Redis-Benchmarks'!$E$91)</definedName>
     <definedName name="tests_1" localSheetId="0">'External Redis-Benchmarks'!$C$12:$J$16</definedName>
     <definedName name="tests_2" localSheetId="0">'External Redis-Benchmarks'!$C$17:$J$20</definedName>
     <definedName name="tests_3" localSheetId="0">'External Redis-Benchmarks'!$C$21:$J$24</definedName>
@@ -623,7 +630,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -641,10 +648,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3165,7 +3172,7 @@
             <c:strRef>
               <c:f>'Internal Redis-Benchmarks'!$B$66:$J$66</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>SGX Secured Redis</c:v>
                 </c:pt>
@@ -9661,13 +9668,13 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>589561</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>101607</xdr:rowOff>
+      <xdr:rowOff>101606</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>555696</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>1096</xdr:rowOff>
+      <xdr:rowOff>15246</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9855,23 +9862,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_2" connectionId="1" xr16:uid="{EE16474F-CCD2-364B-A607-51BAF623E71C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_3" connectionId="2" xr16:uid="{493998F8-C237-CC45-95DE-DE52776EC4BA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_6" connectionId="6" xr16:uid="{F0609839-D860-594D-A6DC-121FFC03226C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_5" connectionId="4" xr16:uid="{F7C01357-A0B7-9C46-A14F-E3A5D11E2DD6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_1" connectionId="5" xr16:uid="{83893D2E-64E6-4141-91BF-17E4FBF6D821}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_2" connectionId="1" xr16:uid="{EE16474F-CCD2-364B-A607-51BAF623E71C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10173,8 +10180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF65E5F0-7FEC-2D44-A2C2-0F5F83647661}">
   <dimension ref="B2:J92"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="U56" sqref="U56"/>
+    <sheetView tabSelected="1" topLeftCell="I33" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="W48" sqref="W48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10274,7 +10281,7 @@
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="38">
+      <c r="B13" s="32">
         <v>1</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -10357,7 +10364,7 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="39"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="10" t="s">
         <v>17</v>
       </c>
@@ -10384,7 +10391,7 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="38">
+      <c r="B17" s="32">
         <v>2</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -10467,7 +10474,7 @@
       </c>
     </row>
     <row r="20" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="39"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="10" t="s">
         <v>17</v>
       </c>
@@ -10494,7 +10501,7 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="38">
+      <c r="B21" s="32">
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -10577,7 +10584,7 @@
       </c>
     </row>
     <row r="24" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="39"/>
+      <c r="B24" s="38"/>
       <c r="C24" s="10" t="s">
         <v>17</v>
       </c>
@@ -10604,7 +10611,7 @@
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="38">
+      <c r="B25" s="32">
         <v>4</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -10687,7 +10694,7 @@
       </c>
     </row>
     <row r="28" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="39"/>
+      <c r="B28" s="38"/>
       <c r="C28" s="10" t="s">
         <v>17</v>
       </c>
@@ -10714,7 +10721,7 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="38">
+      <c r="B29" s="32">
         <v>5</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -10824,7 +10831,7 @@
       </c>
     </row>
     <row r="33" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="39" t="s">
         <v>18</v>
       </c>
       <c r="C33" s="16" t="s">
@@ -11006,7 +11013,7 @@
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="38">
+      <c r="B41" s="32">
         <v>1</v>
       </c>
       <c r="C41" s="8" t="s">
@@ -11089,7 +11096,7 @@
       </c>
     </row>
     <row r="44" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="39"/>
+      <c r="B44" s="38"/>
       <c r="C44" s="10" t="s">
         <v>17</v>
       </c>
@@ -11116,7 +11123,7 @@
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B45" s="38">
+      <c r="B45" s="32">
         <v>2</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -11199,7 +11206,7 @@
       </c>
     </row>
     <row r="48" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="39"/>
+      <c r="B48" s="38"/>
       <c r="C48" s="10" t="s">
         <v>17</v>
       </c>
@@ -11226,7 +11233,7 @@
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B49" s="38">
+      <c r="B49" s="32">
         <v>3</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -11309,7 +11316,7 @@
       </c>
     </row>
     <row r="52" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="39"/>
+      <c r="B52" s="38"/>
       <c r="C52" s="10" t="s">
         <v>17</v>
       </c>
@@ -11336,7 +11343,7 @@
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B53" s="38">
+      <c r="B53" s="32">
         <v>4</v>
       </c>
       <c r="C53" s="8" t="s">
@@ -11419,7 +11426,7 @@
       </c>
     </row>
     <row r="56" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="39"/>
+      <c r="B56" s="38"/>
       <c r="C56" s="10" t="s">
         <v>17</v>
       </c>
@@ -11446,7 +11453,7 @@
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" s="38">
+      <c r="B57" s="32">
         <v>5</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -11556,7 +11563,7 @@
       </c>
     </row>
     <row r="61" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="32" t="s">
+      <c r="B61" s="39" t="s">
         <v>18</v>
       </c>
       <c r="C61" s="16" t="s">
@@ -11737,7 +11744,7 @@
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B68" s="38">
+      <c r="B68" s="32">
         <v>1</v>
       </c>
       <c r="C68" s="8" t="s">
@@ -11820,7 +11827,7 @@
       </c>
     </row>
     <row r="71" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="39"/>
+      <c r="B71" s="38"/>
       <c r="C71" s="10" t="s">
         <v>17</v>
       </c>
@@ -11847,7 +11854,7 @@
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B72" s="38">
+      <c r="B72" s="32">
         <v>2</v>
       </c>
       <c r="C72" s="8" t="s">
@@ -11930,7 +11937,7 @@
       </c>
     </row>
     <row r="75" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="39"/>
+      <c r="B75" s="38"/>
       <c r="C75" s="10" t="s">
         <v>17</v>
       </c>
@@ -11957,7 +11964,7 @@
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B76" s="38">
+      <c r="B76" s="32">
         <v>3</v>
       </c>
       <c r="C76" s="8" t="s">
@@ -12040,7 +12047,7 @@
       </c>
     </row>
     <row r="79" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="39"/>
+      <c r="B79" s="38"/>
       <c r="C79" s="10" t="s">
         <v>17</v>
       </c>
@@ -12067,7 +12074,7 @@
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B80" s="38">
+      <c r="B80" s="32">
         <v>4</v>
       </c>
       <c r="C80" s="8" t="s">
@@ -12150,7 +12157,7 @@
       </c>
     </row>
     <row r="83" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="39"/>
+      <c r="B83" s="38"/>
       <c r="C83" s="10" t="s">
         <v>17</v>
       </c>
@@ -12177,7 +12184,7 @@
       </c>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B84" s="38">
+      <c r="B84" s="32">
         <v>5</v>
       </c>
       <c r="C84" s="8" t="s">
@@ -12287,7 +12294,7 @@
       </c>
     </row>
     <row r="88" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="32" t="s">
+      <c r="B88" s="39" t="s">
         <v>18</v>
       </c>
       <c r="C88" s="16" t="s">
@@ -12427,12 +12434,6 @@
     <row r="92" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="B11:J11"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B25:B28"/>
     <mergeCell ref="B61:B64"/>
     <mergeCell ref="B33:B36"/>
     <mergeCell ref="B88:B91"/>
@@ -12448,6 +12449,12 @@
     <mergeCell ref="B49:B52"/>
     <mergeCell ref="B53:B56"/>
     <mergeCell ref="B57:B60"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B25:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12458,7 +12465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1D7AB5-56EB-A14B-8A61-C582BDE41FCF}">
   <dimension ref="B2:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R26" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AC32" sqref="AC32"/>
     </sheetView>
   </sheetViews>
@@ -12559,7 +12566,7 @@
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="38">
+      <c r="B13" s="32">
         <v>1</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -12642,7 +12649,7 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="39"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="10" t="s">
         <v>17</v>
       </c>
@@ -12669,7 +12676,7 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="38">
+      <c r="B17" s="32">
         <v>2</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -12752,7 +12759,7 @@
       </c>
     </row>
     <row r="20" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="39"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="10" t="s">
         <v>17</v>
       </c>
@@ -12779,7 +12786,7 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="38">
+      <c r="B21" s="32">
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -12862,7 +12869,7 @@
       </c>
     </row>
     <row r="24" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="39"/>
+      <c r="B24" s="38"/>
       <c r="C24" s="10" t="s">
         <v>17</v>
       </c>
@@ -12889,7 +12896,7 @@
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="38">
+      <c r="B25" s="32">
         <v>4</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -12972,7 +12979,7 @@
       </c>
     </row>
     <row r="28" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="39"/>
+      <c r="B28" s="38"/>
       <c r="C28" s="10" t="s">
         <v>17</v>
       </c>
@@ -12999,7 +13006,7 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="38">
+      <c r="B29" s="32">
         <v>5</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -13109,7 +13116,7 @@
       </c>
     </row>
     <row r="33" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="39" t="s">
         <v>18</v>
       </c>
       <c r="C33" s="8" t="s">
@@ -13291,7 +13298,7 @@
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="38">
+      <c r="B41" s="32">
         <v>1</v>
       </c>
       <c r="C41" s="8" t="s">
@@ -13374,7 +13381,7 @@
       </c>
     </row>
     <row r="44" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="39"/>
+      <c r="B44" s="38"/>
       <c r="C44" s="10" t="s">
         <v>17</v>
       </c>
@@ -13401,7 +13408,7 @@
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B45" s="38">
+      <c r="B45" s="32">
         <v>2</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -13484,7 +13491,7 @@
       </c>
     </row>
     <row r="48" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="39"/>
+      <c r="B48" s="38"/>
       <c r="C48" s="10" t="s">
         <v>17</v>
       </c>
@@ -13511,7 +13518,7 @@
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B49" s="38">
+      <c r="B49" s="32">
         <v>3</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -13594,7 +13601,7 @@
       </c>
     </row>
     <row r="52" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="39"/>
+      <c r="B52" s="38"/>
       <c r="C52" s="10" t="s">
         <v>17</v>
       </c>
@@ -13621,7 +13628,7 @@
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B53" s="38">
+      <c r="B53" s="32">
         <v>4</v>
       </c>
       <c r="C53" s="8" t="s">
@@ -13704,7 +13711,7 @@
       </c>
     </row>
     <row r="56" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="39"/>
+      <c r="B56" s="38"/>
       <c r="C56" s="10" t="s">
         <v>17</v>
       </c>
@@ -13731,7 +13738,7 @@
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" s="38">
+      <c r="B57" s="32">
         <v>5</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -13841,7 +13848,7 @@
       </c>
     </row>
     <row r="61" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="32" t="s">
+      <c r="B61" s="39" t="s">
         <v>18</v>
       </c>
       <c r="C61" s="8" t="s">
@@ -14022,7 +14029,7 @@
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B68" s="38">
+      <c r="B68" s="32">
         <v>1</v>
       </c>
       <c r="C68" s="8" t="s">
@@ -14105,7 +14112,7 @@
       </c>
     </row>
     <row r="71" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="39"/>
+      <c r="B71" s="38"/>
       <c r="C71" s="10" t="s">
         <v>17</v>
       </c>
@@ -14132,7 +14139,7 @@
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B72" s="38">
+      <c r="B72" s="32">
         <v>2</v>
       </c>
       <c r="C72" s="8" t="s">
@@ -14215,7 +14222,7 @@
       </c>
     </row>
     <row r="75" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="39"/>
+      <c r="B75" s="38"/>
       <c r="C75" s="10" t="s">
         <v>17</v>
       </c>
@@ -14242,7 +14249,7 @@
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B76" s="38">
+      <c r="B76" s="32">
         <v>3</v>
       </c>
       <c r="C76" s="8" t="s">
@@ -14325,7 +14332,7 @@
       </c>
     </row>
     <row r="79" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="39"/>
+      <c r="B79" s="38"/>
       <c r="C79" s="10" t="s">
         <v>17</v>
       </c>
@@ -14352,7 +14359,7 @@
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B80" s="38">
+      <c r="B80" s="32">
         <v>4</v>
       </c>
       <c r="C80" s="8" t="s">
@@ -14435,7 +14442,7 @@
       </c>
     </row>
     <row r="83" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="39"/>
+      <c r="B83" s="38"/>
       <c r="C83" s="10" t="s">
         <v>17</v>
       </c>
@@ -14462,7 +14469,7 @@
       </c>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B84" s="38">
+      <c r="B84" s="32">
         <v>5</v>
       </c>
       <c r="C84" s="8" t="s">
@@ -14572,7 +14579,7 @@
       </c>
     </row>
     <row r="88" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="32" t="s">
+      <c r="B88" s="39" t="s">
         <v>18</v>
       </c>
       <c r="C88" s="8" t="s">
@@ -14712,6 +14719,15 @@
     <row r="92" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="B66:J66"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="B76:B79"/>
     <mergeCell ref="B53:B56"/>
     <mergeCell ref="B11:J11"/>
     <mergeCell ref="B13:B16"/>
@@ -14724,15 +14740,6 @@
     <mergeCell ref="B41:B44"/>
     <mergeCell ref="B45:B48"/>
     <mergeCell ref="B49:B52"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="B88:B91"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="B66:J66"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="B76:B79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added trhoughput graph example to excel
</commit_message>
<xml_diff>
--- a/thesis-tests.xlsx
+++ b/thesis-tests.xlsx
@@ -8,22 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguelanciaes/Desktop/thesis/novathesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2A5037-7E01-1A4C-BB98-8AFAC46AE352}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDFC7FF-4DF8-3147-A396-AE0619343C8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{6308EBAC-DE62-D645-97F4-0D2E9D77B78B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" activeTab="2" xr2:uid="{6308EBAC-DE62-D645-97F4-0D2E9D77B78B}"/>
   </bookViews>
   <sheets>
     <sheet name="External Redis-Benchmarks" sheetId="2" r:id="rId1"/>
     <sheet name="Internal Redis-Benchmarks" sheetId="3" r:id="rId2"/>
+    <sheet name="Throughput Graphs" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'External Redis-Benchmarks'!$B$11:$J$11</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'External Redis-Benchmarks'!$B$39:$J$39</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'External Redis-Benchmarks'!$B$66:$J$66</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">('External Redis-Benchmarks'!$C$33,'External Redis-Benchmarks'!$C$35,'External Redis-Benchmarks'!$C$36)</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">('External Redis-Benchmarks'!$E$33,'External Redis-Benchmarks'!$E$35,'External Redis-Benchmarks'!$E$36)</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">('External Redis-Benchmarks'!$E$61,'External Redis-Benchmarks'!$E$63,'External Redis-Benchmarks'!$E$64)</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">('External Redis-Benchmarks'!$E$88,'External Redis-Benchmarks'!$E$90,'External Redis-Benchmarks'!$E$91)</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Throughput Graphs'!$C$5</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Throughput Graphs'!$C$6:$C$12</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Throughput Graphs'!$D$5</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Throughput Graphs'!$D$6:$D$12</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">'Throughput Graphs'!$C$5</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">'Throughput Graphs'!$C$6:$C$12</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">'Throughput Graphs'!$D$5</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">'Throughput Graphs'!$D$6:$D$12</definedName>
     <definedName name="tests_1" localSheetId="0">'External Redis-Benchmarks'!$C$12:$J$16</definedName>
     <definedName name="tests_2" localSheetId="0">'External Redis-Benchmarks'!$C$17:$J$20</definedName>
     <definedName name="tests_3" localSheetId="0">'External Redis-Benchmarks'!$C$21:$J$24</definedName>
@@ -139,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="30">
   <si>
     <t>Test Configurations</t>
   </si>
@@ -215,6 +217,21 @@
   <si>
     <t>SGX Secured Redis</t>
   </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Requests</t>
+  </si>
+  <si>
+    <t>GET Throughput</t>
+  </si>
+  <si>
+    <t>Proxy  - Redis</t>
+  </si>
+  <si>
+    <t>Proxy SGX - Redis SGX</t>
+  </si>
 </sst>
 </file>
 
@@ -223,7 +240,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -237,6 +254,14 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -246,7 +271,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -593,11 +618,101 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -630,7 +745,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -648,10 +763,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5824,6 +5951,561 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>GET Throughput</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Throughput Graphs'!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Proxy  - Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Throughput Graphs'!$C$6:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Throughput Graphs'!$D$6:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>321</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>532</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B779-5547-B112-F52CB8C2A4EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Throughput Graphs'!$C$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Proxy SGX - Redis SGX</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Throughput Graphs'!$C$17:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Throughput Graphs'!$D$17:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>543</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>456</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>435</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>234</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B779-5547-B112-F52CB8C2A4EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1553195167"/>
+        <c:axId val="1553196815"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1553195167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1553196815"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1553196815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Operations</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> per Second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1553195167"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -6104,6 +6786,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -9570,6 +10292,522 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -9857,28 +11095,69 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>692150</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90D20599-F8BD-BA43-8CFB-E5411DA46714}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_4" connectionId="3" xr16:uid="{C5EE8FE5-0397-574F-96C7-029D8D92F13D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_1" connectionId="5" xr16:uid="{83893D2E-64E6-4141-91BF-17E4FBF6D821}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_2" connectionId="1" xr16:uid="{EE16474F-CCD2-364B-A607-51BAF623E71C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_3" connectionId="2" xr16:uid="{493998F8-C237-CC45-95DE-DE52776EC4BA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_6" connectionId="6" xr16:uid="{F0609839-D860-594D-A6DC-121FFC03226C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_5" connectionId="4" xr16:uid="{F7C01357-A0B7-9C46-A14F-E3A5D11E2DD6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_1" connectionId="5" xr16:uid="{83893D2E-64E6-4141-91BF-17E4FBF6D821}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10180,7 +11459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF65E5F0-7FEC-2D44-A2C2-0F5F83647661}">
   <dimension ref="B2:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I33" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="I33" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="W48" sqref="W48"/>
     </sheetView>
   </sheetViews>
@@ -10281,7 +11560,7 @@
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="32">
+      <c r="B13" s="38">
         <v>1</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -10364,7 +11643,7 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="38"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="10" t="s">
         <v>17</v>
       </c>
@@ -10391,7 +11670,7 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="32">
+      <c r="B17" s="38">
         <v>2</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -10474,7 +11753,7 @@
       </c>
     </row>
     <row r="20" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="38"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="10" t="s">
         <v>17</v>
       </c>
@@ -10501,7 +11780,7 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="32">
+      <c r="B21" s="38">
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -10584,7 +11863,7 @@
       </c>
     </row>
     <row r="24" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="38"/>
+      <c r="B24" s="39"/>
       <c r="C24" s="10" t="s">
         <v>17</v>
       </c>
@@ -10611,7 +11890,7 @@
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="32">
+      <c r="B25" s="38">
         <v>4</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -10694,7 +11973,7 @@
       </c>
     </row>
     <row r="28" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="38"/>
+      <c r="B28" s="39"/>
       <c r="C28" s="10" t="s">
         <v>17</v>
       </c>
@@ -10721,7 +12000,7 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="32">
+      <c r="B29" s="38">
         <v>5</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -10831,7 +12110,7 @@
       </c>
     </row>
     <row r="33" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C33" s="16" t="s">
@@ -11013,7 +12292,7 @@
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="32">
+      <c r="B41" s="38">
         <v>1</v>
       </c>
       <c r="C41" s="8" t="s">
@@ -11096,7 +12375,7 @@
       </c>
     </row>
     <row r="44" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="38"/>
+      <c r="B44" s="39"/>
       <c r="C44" s="10" t="s">
         <v>17</v>
       </c>
@@ -11123,7 +12402,7 @@
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B45" s="32">
+      <c r="B45" s="38">
         <v>2</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -11206,7 +12485,7 @@
       </c>
     </row>
     <row r="48" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="38"/>
+      <c r="B48" s="39"/>
       <c r="C48" s="10" t="s">
         <v>17</v>
       </c>
@@ -11233,7 +12512,7 @@
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B49" s="32">
+      <c r="B49" s="38">
         <v>3</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -11316,7 +12595,7 @@
       </c>
     </row>
     <row r="52" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="38"/>
+      <c r="B52" s="39"/>
       <c r="C52" s="10" t="s">
         <v>17</v>
       </c>
@@ -11343,7 +12622,7 @@
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B53" s="32">
+      <c r="B53" s="38">
         <v>4</v>
       </c>
       <c r="C53" s="8" t="s">
@@ -11426,7 +12705,7 @@
       </c>
     </row>
     <row r="56" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="38"/>
+      <c r="B56" s="39"/>
       <c r="C56" s="10" t="s">
         <v>17</v>
       </c>
@@ -11453,7 +12732,7 @@
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" s="32">
+      <c r="B57" s="38">
         <v>5</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -11563,7 +12842,7 @@
       </c>
     </row>
     <row r="61" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="39" t="s">
+      <c r="B61" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C61" s="16" t="s">
@@ -11744,7 +13023,7 @@
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B68" s="32">
+      <c r="B68" s="38">
         <v>1</v>
       </c>
       <c r="C68" s="8" t="s">
@@ -11827,7 +13106,7 @@
       </c>
     </row>
     <row r="71" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="38"/>
+      <c r="B71" s="39"/>
       <c r="C71" s="10" t="s">
         <v>17</v>
       </c>
@@ -11854,7 +13133,7 @@
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B72" s="32">
+      <c r="B72" s="38">
         <v>2</v>
       </c>
       <c r="C72" s="8" t="s">
@@ -11937,7 +13216,7 @@
       </c>
     </row>
     <row r="75" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="38"/>
+      <c r="B75" s="39"/>
       <c r="C75" s="10" t="s">
         <v>17</v>
       </c>
@@ -11964,7 +13243,7 @@
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B76" s="32">
+      <c r="B76" s="38">
         <v>3</v>
       </c>
       <c r="C76" s="8" t="s">
@@ -12047,7 +13326,7 @@
       </c>
     </row>
     <row r="79" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="38"/>
+      <c r="B79" s="39"/>
       <c r="C79" s="10" t="s">
         <v>17</v>
       </c>
@@ -12074,7 +13353,7 @@
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B80" s="32">
+      <c r="B80" s="38">
         <v>4</v>
       </c>
       <c r="C80" s="8" t="s">
@@ -12157,7 +13436,7 @@
       </c>
     </row>
     <row r="83" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="38"/>
+      <c r="B83" s="39"/>
       <c r="C83" s="10" t="s">
         <v>17</v>
       </c>
@@ -12184,7 +13463,7 @@
       </c>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B84" s="32">
+      <c r="B84" s="38">
         <v>5</v>
       </c>
       <c r="C84" s="8" t="s">
@@ -12294,7 +13573,7 @@
       </c>
     </row>
     <row r="88" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="39" t="s">
+      <c r="B88" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C88" s="16" t="s">
@@ -12434,6 +13713,12 @@
     <row r="92" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B25:B28"/>
     <mergeCell ref="B61:B64"/>
     <mergeCell ref="B33:B36"/>
     <mergeCell ref="B88:B91"/>
@@ -12449,12 +13734,6 @@
     <mergeCell ref="B49:B52"/>
     <mergeCell ref="B53:B56"/>
     <mergeCell ref="B57:B60"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="B11:J11"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B25:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12566,7 +13845,7 @@
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="32">
+      <c r="B13" s="38">
         <v>1</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -12649,7 +13928,7 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="38"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="10" t="s">
         <v>17</v>
       </c>
@@ -12676,7 +13955,7 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="32">
+      <c r="B17" s="38">
         <v>2</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -12759,7 +14038,7 @@
       </c>
     </row>
     <row r="20" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="38"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="10" t="s">
         <v>17</v>
       </c>
@@ -12786,7 +14065,7 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="32">
+      <c r="B21" s="38">
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -12869,7 +14148,7 @@
       </c>
     </row>
     <row r="24" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="38"/>
+      <c r="B24" s="39"/>
       <c r="C24" s="10" t="s">
         <v>17</v>
       </c>
@@ -12896,7 +14175,7 @@
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="32">
+      <c r="B25" s="38">
         <v>4</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -12979,7 +14258,7 @@
       </c>
     </row>
     <row r="28" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="38"/>
+      <c r="B28" s="39"/>
       <c r="C28" s="10" t="s">
         <v>17</v>
       </c>
@@ -13006,7 +14285,7 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="32">
+      <c r="B29" s="38">
         <v>5</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -13116,7 +14395,7 @@
       </c>
     </row>
     <row r="33" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C33" s="8" t="s">
@@ -13298,7 +14577,7 @@
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="32">
+      <c r="B41" s="38">
         <v>1</v>
       </c>
       <c r="C41" s="8" t="s">
@@ -13381,7 +14660,7 @@
       </c>
     </row>
     <row r="44" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="38"/>
+      <c r="B44" s="39"/>
       <c r="C44" s="10" t="s">
         <v>17</v>
       </c>
@@ -13408,7 +14687,7 @@
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B45" s="32">
+      <c r="B45" s="38">
         <v>2</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -13491,7 +14770,7 @@
       </c>
     </row>
     <row r="48" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="38"/>
+      <c r="B48" s="39"/>
       <c r="C48" s="10" t="s">
         <v>17</v>
       </c>
@@ -13518,7 +14797,7 @@
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B49" s="32">
+      <c r="B49" s="38">
         <v>3</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -13601,7 +14880,7 @@
       </c>
     </row>
     <row r="52" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="38"/>
+      <c r="B52" s="39"/>
       <c r="C52" s="10" t="s">
         <v>17</v>
       </c>
@@ -13628,7 +14907,7 @@
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B53" s="32">
+      <c r="B53" s="38">
         <v>4</v>
       </c>
       <c r="C53" s="8" t="s">
@@ -13711,7 +14990,7 @@
       </c>
     </row>
     <row r="56" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="38"/>
+      <c r="B56" s="39"/>
       <c r="C56" s="10" t="s">
         <v>17</v>
       </c>
@@ -13738,7 +15017,7 @@
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" s="32">
+      <c r="B57" s="38">
         <v>5</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -13848,7 +15127,7 @@
       </c>
     </row>
     <row r="61" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="39" t="s">
+      <c r="B61" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C61" s="8" t="s">
@@ -14029,7 +15308,7 @@
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B68" s="32">
+      <c r="B68" s="38">
         <v>1</v>
       </c>
       <c r="C68" s="8" t="s">
@@ -14112,7 +15391,7 @@
       </c>
     </row>
     <row r="71" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="38"/>
+      <c r="B71" s="39"/>
       <c r="C71" s="10" t="s">
         <v>17</v>
       </c>
@@ -14139,7 +15418,7 @@
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B72" s="32">
+      <c r="B72" s="38">
         <v>2</v>
       </c>
       <c r="C72" s="8" t="s">
@@ -14222,7 +15501,7 @@
       </c>
     </row>
     <row r="75" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="38"/>
+      <c r="B75" s="39"/>
       <c r="C75" s="10" t="s">
         <v>17</v>
       </c>
@@ -14249,7 +15528,7 @@
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B76" s="32">
+      <c r="B76" s="38">
         <v>3</v>
       </c>
       <c r="C76" s="8" t="s">
@@ -14332,7 +15611,7 @@
       </c>
     </row>
     <row r="79" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="38"/>
+      <c r="B79" s="39"/>
       <c r="C79" s="10" t="s">
         <v>17</v>
       </c>
@@ -14359,7 +15638,7 @@
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B80" s="32">
+      <c r="B80" s="38">
         <v>4</v>
       </c>
       <c r="C80" s="8" t="s">
@@ -14442,7 +15721,7 @@
       </c>
     </row>
     <row r="83" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="38"/>
+      <c r="B83" s="39"/>
       <c r="C83" s="10" t="s">
         <v>17</v>
       </c>
@@ -14469,7 +15748,7 @@
       </c>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B84" s="32">
+      <c r="B84" s="38">
         <v>5</v>
       </c>
       <c r="C84" s="8" t="s">
@@ -14579,7 +15858,7 @@
       </c>
     </row>
     <row r="88" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="39" t="s">
+      <c r="B88" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C88" s="8" t="s">
@@ -14719,15 +15998,6 @@
     <row r="92" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="B88:B91"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="B66:J66"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="B76:B79"/>
     <mergeCell ref="B53:B56"/>
     <mergeCell ref="B11:J11"/>
     <mergeCell ref="B13:B16"/>
@@ -14740,6 +16010,186 @@
     <mergeCell ref="B41:B44"/>
     <mergeCell ref="B45:B48"/>
     <mergeCell ref="B49:B52"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="B66:J66"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="B76:B79"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{074A9C4C-98EA-374F-B3FE-F455AC9FA99B}">
+  <dimension ref="C2:D24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C2" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="40"/>
+    </row>
+    <row r="3" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="3:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="37"/>
+    </row>
+    <row r="5" spans="3:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="43">
+        <v>0</v>
+      </c>
+      <c r="D6" s="44">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="43">
+        <v>1</v>
+      </c>
+      <c r="D7" s="44">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="43">
+        <v>2</v>
+      </c>
+      <c r="D8" s="44">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="43">
+        <v>3</v>
+      </c>
+      <c r="D9" s="44">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="43">
+        <v>4</v>
+      </c>
+      <c r="D10" s="44">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="43">
+        <v>5</v>
+      </c>
+      <c r="D11" s="44">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="45">
+        <v>6</v>
+      </c>
+      <c r="D12" s="46">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="3:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="37"/>
+    </row>
+    <row r="16" spans="3:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="43">
+        <v>0</v>
+      </c>
+      <c r="D17" s="44">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="43">
+        <v>1</v>
+      </c>
+      <c r="D18" s="44">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="43">
+        <v>2</v>
+      </c>
+      <c r="D19" s="44">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="43">
+        <v>3</v>
+      </c>
+      <c r="D20" s="44">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="43">
+        <v>4</v>
+      </c>
+      <c r="D21" s="44">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="43">
+        <v>5</v>
+      </c>
+      <c r="D22" s="44">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="45">
+        <v>6</v>
+      </c>
+      <c r="D23" s="46">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Updated homomorphic encryption search results with better internet. Added attestation response example to annex
</commit_message>
<xml_diff>
--- a/thesis-tests.xlsx
+++ b/thesis-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguelanciaes/Desktop/thesis/novathesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4751A5E1-FE34-E148-85FB-B54DE0DA27DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424B498C-1B30-BD43-B99B-B09BFAB6415C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{6308EBAC-DE62-D645-97F4-0D2E9D77B78B}"/>
   </bookViews>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="81">
   <si>
     <t>Test Configurations</t>
   </si>
@@ -370,6 +370,15 @@
   <si>
     <t>Search Homomorphic Encryption</t>
   </si>
+  <si>
+    <t>0.2MB</t>
+  </si>
+  <si>
+    <t>0.49MB</t>
+  </si>
+  <si>
+    <t>0.27MB</t>
+  </si>
 </sst>
 </file>
 
@@ -418,7 +427,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="53">
+  <borders count="55">
     <border>
       <left/>
       <right/>
@@ -1096,11 +1105,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1265,9 +1300,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1288,7 +1320,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1306,10 +1344,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1341,7 +1379,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2985,37 +3032,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3115,31 +3162,31 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3233,13 +3280,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10</c:v>
@@ -3248,19 +3295,19 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>9</c:v>
@@ -16204,23 +16251,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_2" connectionId="1" xr16:uid="{EE16474F-CCD2-364B-A607-51BAF623E71C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_3" connectionId="2" xr16:uid="{493998F8-C237-CC45-95DE-DE52776EC4BA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_6" connectionId="6" xr16:uid="{F0609839-D860-594D-A6DC-121FFC03226C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_5" connectionId="4" xr16:uid="{F7C01357-A0B7-9C46-A14F-E3A5D11E2DD6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_1" connectionId="5" xr16:uid="{83893D2E-64E6-4141-91BF-17E4FBF6D821}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_2" connectionId="1" xr16:uid="{EE16474F-CCD2-364B-A607-51BAF623E71C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16581,17 +16628,17 @@
       <c r="B10" s="6"/>
     </row>
     <row r="11" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="94" t="s">
+      <c r="B11" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="95"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="95"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="95"/>
-      <c r="I11" s="95"/>
-      <c r="J11" s="96"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
+      <c r="H11" s="96"/>
+      <c r="I11" s="96"/>
+      <c r="J11" s="97"/>
     </row>
     <row r="12" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
@@ -16623,7 +16670,7 @@
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="91">
+      <c r="B13" s="98">
         <v>1</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -16652,7 +16699,7 @@
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="92"/>
+      <c r="B14" s="93"/>
       <c r="C14" s="9" t="s">
         <v>15</v>
       </c>
@@ -16679,7 +16726,7 @@
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="92"/>
+      <c r="B15" s="93"/>
       <c r="C15" s="9" t="s">
         <v>16</v>
       </c>
@@ -16706,7 +16753,7 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="97"/>
+      <c r="B16" s="99"/>
       <c r="C16" s="10" t="s">
         <v>17</v>
       </c>
@@ -16733,7 +16780,7 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="91">
+      <c r="B17" s="98">
         <v>2</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -16762,7 +16809,7 @@
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="92"/>
+      <c r="B18" s="93"/>
       <c r="C18" s="9" t="s">
         <v>15</v>
       </c>
@@ -16789,7 +16836,7 @@
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="92"/>
+      <c r="B19" s="93"/>
       <c r="C19" s="9" t="s">
         <v>16</v>
       </c>
@@ -16816,7 +16863,7 @@
       </c>
     </row>
     <row r="20" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="97"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="10" t="s">
         <v>17</v>
       </c>
@@ -16843,7 +16890,7 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="91">
+      <c r="B21" s="98">
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -16872,7 +16919,7 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="92"/>
+      <c r="B22" s="93"/>
       <c r="C22" s="9" t="s">
         <v>15</v>
       </c>
@@ -16899,7 +16946,7 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="92"/>
+      <c r="B23" s="93"/>
       <c r="C23" s="9" t="s">
         <v>16</v>
       </c>
@@ -16926,7 +16973,7 @@
       </c>
     </row>
     <row r="24" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="97"/>
+      <c r="B24" s="99"/>
       <c r="C24" s="10" t="s">
         <v>17</v>
       </c>
@@ -16953,7 +17000,7 @@
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="91">
+      <c r="B25" s="98">
         <v>4</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -16982,7 +17029,7 @@
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B26" s="92"/>
+      <c r="B26" s="93"/>
       <c r="C26" s="9" t="s">
         <v>15</v>
       </c>
@@ -17009,7 +17056,7 @@
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="92"/>
+      <c r="B27" s="93"/>
       <c r="C27" s="9" t="s">
         <v>16</v>
       </c>
@@ -17036,7 +17083,7 @@
       </c>
     </row>
     <row r="28" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="97"/>
+      <c r="B28" s="99"/>
       <c r="C28" s="10" t="s">
         <v>17</v>
       </c>
@@ -17063,7 +17110,7 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="91">
+      <c r="B29" s="98">
         <v>5</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -17092,7 +17139,7 @@
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B30" s="92"/>
+      <c r="B30" s="93"/>
       <c r="C30" s="9" t="s">
         <v>15</v>
       </c>
@@ -17119,7 +17166,7 @@
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B31" s="92"/>
+      <c r="B31" s="93"/>
       <c r="C31" s="9" t="s">
         <v>16</v>
       </c>
@@ -17146,7 +17193,7 @@
       </c>
     </row>
     <row r="32" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="93"/>
+      <c r="B32" s="94"/>
       <c r="C32" s="14" t="s">
         <v>17</v>
       </c>
@@ -17173,7 +17220,7 @@
       </c>
     </row>
     <row r="33" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="98" t="s">
+      <c r="B33" s="92" t="s">
         <v>18</v>
       </c>
       <c r="C33" s="16" t="s">
@@ -17209,7 +17256,7 @@
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="92"/>
+      <c r="B34" s="93"/>
       <c r="C34" s="9" t="s">
         <v>15</v>
       </c>
@@ -17243,7 +17290,7 @@
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B35" s="92"/>
+      <c r="B35" s="93"/>
       <c r="C35" s="9" t="s">
         <v>20</v>
       </c>
@@ -17277,7 +17324,7 @@
       </c>
     </row>
     <row r="36" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="93"/>
+      <c r="B36" s="94"/>
       <c r="C36" s="14" t="s">
         <v>21</v>
       </c>
@@ -17313,17 +17360,17 @@
     <row r="37" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="94" t="s">
+      <c r="B39" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="95"/>
-      <c r="D39" s="95"/>
-      <c r="E39" s="95"/>
-      <c r="F39" s="95"/>
-      <c r="G39" s="95"/>
-      <c r="H39" s="95"/>
-      <c r="I39" s="95"/>
-      <c r="J39" s="96"/>
+      <c r="C39" s="96"/>
+      <c r="D39" s="96"/>
+      <c r="E39" s="96"/>
+      <c r="F39" s="96"/>
+      <c r="G39" s="96"/>
+      <c r="H39" s="96"/>
+      <c r="I39" s="96"/>
+      <c r="J39" s="97"/>
     </row>
     <row r="40" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="26" t="s">
@@ -17355,7 +17402,7 @@
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="91">
+      <c r="B41" s="98">
         <v>1</v>
       </c>
       <c r="C41" s="8" t="s">
@@ -17384,7 +17431,7 @@
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B42" s="92"/>
+      <c r="B42" s="93"/>
       <c r="C42" s="9" t="s">
         <v>15</v>
       </c>
@@ -17411,7 +17458,7 @@
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B43" s="92"/>
+      <c r="B43" s="93"/>
       <c r="C43" s="9" t="s">
         <v>16</v>
       </c>
@@ -17438,7 +17485,7 @@
       </c>
     </row>
     <row r="44" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="97"/>
+      <c r="B44" s="99"/>
       <c r="C44" s="10" t="s">
         <v>17</v>
       </c>
@@ -17465,7 +17512,7 @@
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B45" s="91">
+      <c r="B45" s="98">
         <v>2</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -17494,7 +17541,7 @@
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B46" s="92"/>
+      <c r="B46" s="93"/>
       <c r="C46" s="9" t="s">
         <v>15</v>
       </c>
@@ -17521,7 +17568,7 @@
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B47" s="92"/>
+      <c r="B47" s="93"/>
       <c r="C47" s="9" t="s">
         <v>16</v>
       </c>
@@ -17548,7 +17595,7 @@
       </c>
     </row>
     <row r="48" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="97"/>
+      <c r="B48" s="99"/>
       <c r="C48" s="10" t="s">
         <v>17</v>
       </c>
@@ -17575,7 +17622,7 @@
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B49" s="91">
+      <c r="B49" s="98">
         <v>3</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -17604,7 +17651,7 @@
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B50" s="92"/>
+      <c r="B50" s="93"/>
       <c r="C50" s="9" t="s">
         <v>15</v>
       </c>
@@ -17631,7 +17678,7 @@
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B51" s="92"/>
+      <c r="B51" s="93"/>
       <c r="C51" s="9" t="s">
         <v>16</v>
       </c>
@@ -17658,7 +17705,7 @@
       </c>
     </row>
     <row r="52" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="97"/>
+      <c r="B52" s="99"/>
       <c r="C52" s="10" t="s">
         <v>17</v>
       </c>
@@ -17685,7 +17732,7 @@
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B53" s="91">
+      <c r="B53" s="98">
         <v>4</v>
       </c>
       <c r="C53" s="8" t="s">
@@ -17714,7 +17761,7 @@
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B54" s="92"/>
+      <c r="B54" s="93"/>
       <c r="C54" s="9" t="s">
         <v>15</v>
       </c>
@@ -17741,7 +17788,7 @@
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B55" s="92"/>
+      <c r="B55" s="93"/>
       <c r="C55" s="9" t="s">
         <v>16</v>
       </c>
@@ -17768,7 +17815,7 @@
       </c>
     </row>
     <row r="56" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="97"/>
+      <c r="B56" s="99"/>
       <c r="C56" s="10" t="s">
         <v>17</v>
       </c>
@@ -17795,7 +17842,7 @@
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" s="91">
+      <c r="B57" s="98">
         <v>5</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -17824,7 +17871,7 @@
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B58" s="92"/>
+      <c r="B58" s="93"/>
       <c r="C58" s="9" t="s">
         <v>15</v>
       </c>
@@ -17851,7 +17898,7 @@
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B59" s="92"/>
+      <c r="B59" s="93"/>
       <c r="C59" s="9" t="s">
         <v>16</v>
       </c>
@@ -17878,7 +17925,7 @@
       </c>
     </row>
     <row r="60" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="93"/>
+      <c r="B60" s="94"/>
       <c r="C60" s="14" t="s">
         <v>17</v>
       </c>
@@ -17905,7 +17952,7 @@
       </c>
     </row>
     <row r="61" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="98" t="s">
+      <c r="B61" s="92" t="s">
         <v>18</v>
       </c>
       <c r="C61" s="16" t="s">
@@ -17941,7 +17988,7 @@
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B62" s="92"/>
+      <c r="B62" s="93"/>
       <c r="C62" s="9" t="s">
         <v>15</v>
       </c>
@@ -17975,7 +18022,7 @@
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B63" s="92"/>
+      <c r="B63" s="93"/>
       <c r="C63" s="9" t="s">
         <v>16</v>
       </c>
@@ -18009,7 +18056,7 @@
       </c>
     </row>
     <row r="64" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="93"/>
+      <c r="B64" s="94"/>
       <c r="C64" s="14" t="s">
         <v>17</v>
       </c>
@@ -18044,17 +18091,17 @@
     </row>
     <row r="65" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="94" t="s">
+      <c r="B66" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="C66" s="95"/>
-      <c r="D66" s="95"/>
-      <c r="E66" s="95"/>
-      <c r="F66" s="95"/>
-      <c r="G66" s="95"/>
-      <c r="H66" s="95"/>
-      <c r="I66" s="95"/>
-      <c r="J66" s="96"/>
+      <c r="C66" s="96"/>
+      <c r="D66" s="96"/>
+      <c r="E66" s="96"/>
+      <c r="F66" s="96"/>
+      <c r="G66" s="96"/>
+      <c r="H66" s="96"/>
+      <c r="I66" s="96"/>
+      <c r="J66" s="97"/>
     </row>
     <row r="67" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B67" s="26" t="s">
@@ -18086,7 +18133,7 @@
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B68" s="91">
+      <c r="B68" s="98">
         <v>1</v>
       </c>
       <c r="C68" s="8" t="s">
@@ -18115,7 +18162,7 @@
       </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B69" s="92"/>
+      <c r="B69" s="93"/>
       <c r="C69" s="9" t="s">
         <v>15</v>
       </c>
@@ -18142,7 +18189,7 @@
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B70" s="92"/>
+      <c r="B70" s="93"/>
       <c r="C70" s="9" t="s">
         <v>16</v>
       </c>
@@ -18169,7 +18216,7 @@
       </c>
     </row>
     <row r="71" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="97"/>
+      <c r="B71" s="99"/>
       <c r="C71" s="10" t="s">
         <v>17</v>
       </c>
@@ -18196,7 +18243,7 @@
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B72" s="91">
+      <c r="B72" s="98">
         <v>2</v>
       </c>
       <c r="C72" s="8" t="s">
@@ -18225,7 +18272,7 @@
       </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B73" s="92"/>
+      <c r="B73" s="93"/>
       <c r="C73" s="9" t="s">
         <v>15</v>
       </c>
@@ -18252,7 +18299,7 @@
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B74" s="92"/>
+      <c r="B74" s="93"/>
       <c r="C74" s="9" t="s">
         <v>16</v>
       </c>
@@ -18279,7 +18326,7 @@
       </c>
     </row>
     <row r="75" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="97"/>
+      <c r="B75" s="99"/>
       <c r="C75" s="10" t="s">
         <v>17</v>
       </c>
@@ -18306,7 +18353,7 @@
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B76" s="91">
+      <c r="B76" s="98">
         <v>3</v>
       </c>
       <c r="C76" s="8" t="s">
@@ -18335,7 +18382,7 @@
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B77" s="92"/>
+      <c r="B77" s="93"/>
       <c r="C77" s="9" t="s">
         <v>15</v>
       </c>
@@ -18362,7 +18409,7 @@
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B78" s="92"/>
+      <c r="B78" s="93"/>
       <c r="C78" s="9" t="s">
         <v>16</v>
       </c>
@@ -18389,7 +18436,7 @@
       </c>
     </row>
     <row r="79" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="97"/>
+      <c r="B79" s="99"/>
       <c r="C79" s="10" t="s">
         <v>17</v>
       </c>
@@ -18416,7 +18463,7 @@
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B80" s="91">
+      <c r="B80" s="98">
         <v>4</v>
       </c>
       <c r="C80" s="8" t="s">
@@ -18445,7 +18492,7 @@
       </c>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B81" s="92"/>
+      <c r="B81" s="93"/>
       <c r="C81" s="9" t="s">
         <v>15</v>
       </c>
@@ -18472,7 +18519,7 @@
       </c>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B82" s="92"/>
+      <c r="B82" s="93"/>
       <c r="C82" s="9" t="s">
         <v>16</v>
       </c>
@@ -18499,7 +18546,7 @@
       </c>
     </row>
     <row r="83" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="97"/>
+      <c r="B83" s="99"/>
       <c r="C83" s="10" t="s">
         <v>17</v>
       </c>
@@ -18526,7 +18573,7 @@
       </c>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B84" s="91">
+      <c r="B84" s="98">
         <v>5</v>
       </c>
       <c r="C84" s="8" t="s">
@@ -18555,7 +18602,7 @@
       </c>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B85" s="92"/>
+      <c r="B85" s="93"/>
       <c r="C85" s="9" t="s">
         <v>15</v>
       </c>
@@ -18582,7 +18629,7 @@
       </c>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B86" s="92"/>
+      <c r="B86" s="93"/>
       <c r="C86" s="9" t="s">
         <v>16</v>
       </c>
@@ -18609,7 +18656,7 @@
       </c>
     </row>
     <row r="87" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="93"/>
+      <c r="B87" s="94"/>
       <c r="C87" s="14" t="s">
         <v>17</v>
       </c>
@@ -18636,7 +18683,7 @@
       </c>
     </row>
     <row r="88" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="98" t="s">
+      <c r="B88" s="92" t="s">
         <v>18</v>
       </c>
       <c r="C88" s="16" t="s">
@@ -18672,7 +18719,7 @@
       </c>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B89" s="92"/>
+      <c r="B89" s="93"/>
       <c r="C89" s="9" t="s">
         <v>15</v>
       </c>
@@ -18706,7 +18753,7 @@
       </c>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B90" s="92"/>
+      <c r="B90" s="93"/>
       <c r="C90" s="9" t="s">
         <v>16</v>
       </c>
@@ -18740,7 +18787,7 @@
       </c>
     </row>
     <row r="91" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="93"/>
+      <c r="B91" s="94"/>
       <c r="C91" s="14" t="s">
         <v>17</v>
       </c>
@@ -18776,6 +18823,12 @@
     <row r="92" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B25:B28"/>
     <mergeCell ref="B61:B64"/>
     <mergeCell ref="B33:B36"/>
     <mergeCell ref="B88:B91"/>
@@ -18791,12 +18844,6 @@
     <mergeCell ref="B49:B52"/>
     <mergeCell ref="B53:B56"/>
     <mergeCell ref="B57:B60"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="B11:J11"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B25:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -18866,17 +18913,17 @@
       <c r="B10" s="6"/>
     </row>
     <row r="11" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="94" t="s">
+      <c r="B11" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="95"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="95"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="95"/>
-      <c r="I11" s="95"/>
-      <c r="J11" s="96"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
+      <c r="H11" s="96"/>
+      <c r="I11" s="96"/>
+      <c r="J11" s="97"/>
     </row>
     <row r="12" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
@@ -18908,7 +18955,7 @@
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="91">
+      <c r="B13" s="98">
         <v>1</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -18937,7 +18984,7 @@
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="92"/>
+      <c r="B14" s="93"/>
       <c r="C14" s="9" t="s">
         <v>15</v>
       </c>
@@ -18964,7 +19011,7 @@
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="92"/>
+      <c r="B15" s="93"/>
       <c r="C15" s="9" t="s">
         <v>16</v>
       </c>
@@ -18991,7 +19038,7 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="97"/>
+      <c r="B16" s="99"/>
       <c r="C16" s="10" t="s">
         <v>17</v>
       </c>
@@ -19018,7 +19065,7 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="91">
+      <c r="B17" s="98">
         <v>2</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -19047,7 +19094,7 @@
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="92"/>
+      <c r="B18" s="93"/>
       <c r="C18" s="9" t="s">
         <v>15</v>
       </c>
@@ -19074,7 +19121,7 @@
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="92"/>
+      <c r="B19" s="93"/>
       <c r="C19" s="9" t="s">
         <v>16</v>
       </c>
@@ -19101,7 +19148,7 @@
       </c>
     </row>
     <row r="20" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="97"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="10" t="s">
         <v>17</v>
       </c>
@@ -19128,7 +19175,7 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="91">
+      <c r="B21" s="98">
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -19157,7 +19204,7 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="92"/>
+      <c r="B22" s="93"/>
       <c r="C22" s="9" t="s">
         <v>15</v>
       </c>
@@ -19184,7 +19231,7 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="92"/>
+      <c r="B23" s="93"/>
       <c r="C23" s="9" t="s">
         <v>16</v>
       </c>
@@ -19211,7 +19258,7 @@
       </c>
     </row>
     <row r="24" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="97"/>
+      <c r="B24" s="99"/>
       <c r="C24" s="10" t="s">
         <v>17</v>
       </c>
@@ -19238,7 +19285,7 @@
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="91">
+      <c r="B25" s="98">
         <v>4</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -19267,7 +19314,7 @@
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B26" s="92"/>
+      <c r="B26" s="93"/>
       <c r="C26" s="9" t="s">
         <v>15</v>
       </c>
@@ -19294,7 +19341,7 @@
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="92"/>
+      <c r="B27" s="93"/>
       <c r="C27" s="9" t="s">
         <v>16</v>
       </c>
@@ -19321,7 +19368,7 @@
       </c>
     </row>
     <row r="28" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="97"/>
+      <c r="B28" s="99"/>
       <c r="C28" s="10" t="s">
         <v>17</v>
       </c>
@@ -19348,7 +19395,7 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="91">
+      <c r="B29" s="98">
         <v>5</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -19377,7 +19424,7 @@
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B30" s="92"/>
+      <c r="B30" s="93"/>
       <c r="C30" s="9" t="s">
         <v>15</v>
       </c>
@@ -19404,7 +19451,7 @@
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B31" s="92"/>
+      <c r="B31" s="93"/>
       <c r="C31" s="9" t="s">
         <v>16</v>
       </c>
@@ -19431,7 +19478,7 @@
       </c>
     </row>
     <row r="32" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="93"/>
+      <c r="B32" s="94"/>
       <c r="C32" s="14" t="s">
         <v>17</v>
       </c>
@@ -19458,7 +19505,7 @@
       </c>
     </row>
     <row r="33" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="98" t="s">
+      <c r="B33" s="92" t="s">
         <v>18</v>
       </c>
       <c r="C33" s="8" t="s">
@@ -19494,7 +19541,7 @@
       </c>
     </row>
     <row r="34" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="92"/>
+      <c r="B34" s="93"/>
       <c r="C34" s="9" t="s">
         <v>15</v>
       </c>
@@ -19528,7 +19575,7 @@
       </c>
     </row>
     <row r="35" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="92"/>
+      <c r="B35" s="93"/>
       <c r="C35" s="9" t="s">
         <v>20</v>
       </c>
@@ -19562,7 +19609,7 @@
       </c>
     </row>
     <row r="36" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="93"/>
+      <c r="B36" s="94"/>
       <c r="C36" s="14" t="s">
         <v>21</v>
       </c>
@@ -19598,17 +19645,17 @@
     <row r="37" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="94" t="s">
+      <c r="B39" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="95"/>
-      <c r="D39" s="95"/>
-      <c r="E39" s="95"/>
-      <c r="F39" s="95"/>
-      <c r="G39" s="95"/>
-      <c r="H39" s="95"/>
-      <c r="I39" s="95"/>
-      <c r="J39" s="96"/>
+      <c r="C39" s="96"/>
+      <c r="D39" s="96"/>
+      <c r="E39" s="96"/>
+      <c r="F39" s="96"/>
+      <c r="G39" s="96"/>
+      <c r="H39" s="96"/>
+      <c r="I39" s="96"/>
+      <c r="J39" s="97"/>
     </row>
     <row r="40" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="26" t="s">
@@ -19640,7 +19687,7 @@
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="91">
+      <c r="B41" s="98">
         <v>1</v>
       </c>
       <c r="C41" s="8" t="s">
@@ -19669,7 +19716,7 @@
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B42" s="92"/>
+      <c r="B42" s="93"/>
       <c r="C42" s="9" t="s">
         <v>15</v>
       </c>
@@ -19696,7 +19743,7 @@
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B43" s="92"/>
+      <c r="B43" s="93"/>
       <c r="C43" s="9" t="s">
         <v>16</v>
       </c>
@@ -19723,7 +19770,7 @@
       </c>
     </row>
     <row r="44" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="97"/>
+      <c r="B44" s="99"/>
       <c r="C44" s="10" t="s">
         <v>17</v>
       </c>
@@ -19750,7 +19797,7 @@
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B45" s="91">
+      <c r="B45" s="98">
         <v>2</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -19779,7 +19826,7 @@
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B46" s="92"/>
+      <c r="B46" s="93"/>
       <c r="C46" s="9" t="s">
         <v>15</v>
       </c>
@@ -19806,7 +19853,7 @@
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B47" s="92"/>
+      <c r="B47" s="93"/>
       <c r="C47" s="9" t="s">
         <v>16</v>
       </c>
@@ -19833,7 +19880,7 @@
       </c>
     </row>
     <row r="48" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="97"/>
+      <c r="B48" s="99"/>
       <c r="C48" s="10" t="s">
         <v>17</v>
       </c>
@@ -19860,7 +19907,7 @@
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B49" s="91">
+      <c r="B49" s="98">
         <v>3</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -19889,7 +19936,7 @@
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B50" s="92"/>
+      <c r="B50" s="93"/>
       <c r="C50" s="9" t="s">
         <v>15</v>
       </c>
@@ -19916,7 +19963,7 @@
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B51" s="92"/>
+      <c r="B51" s="93"/>
       <c r="C51" s="9" t="s">
         <v>16</v>
       </c>
@@ -19943,7 +19990,7 @@
       </c>
     </row>
     <row r="52" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="97"/>
+      <c r="B52" s="99"/>
       <c r="C52" s="10" t="s">
         <v>17</v>
       </c>
@@ -19970,7 +20017,7 @@
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B53" s="91">
+      <c r="B53" s="98">
         <v>4</v>
       </c>
       <c r="C53" s="8" t="s">
@@ -19999,7 +20046,7 @@
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B54" s="92"/>
+      <c r="B54" s="93"/>
       <c r="C54" s="9" t="s">
         <v>15</v>
       </c>
@@ -20026,7 +20073,7 @@
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B55" s="92"/>
+      <c r="B55" s="93"/>
       <c r="C55" s="9" t="s">
         <v>16</v>
       </c>
@@ -20053,7 +20100,7 @@
       </c>
     </row>
     <row r="56" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="97"/>
+      <c r="B56" s="99"/>
       <c r="C56" s="10" t="s">
         <v>17</v>
       </c>
@@ -20080,7 +20127,7 @@
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" s="91">
+      <c r="B57" s="98">
         <v>5</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -20109,7 +20156,7 @@
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B58" s="92"/>
+      <c r="B58" s="93"/>
       <c r="C58" s="9" t="s">
         <v>15</v>
       </c>
@@ -20136,7 +20183,7 @@
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B59" s="92"/>
+      <c r="B59" s="93"/>
       <c r="C59" s="9" t="s">
         <v>16</v>
       </c>
@@ -20163,7 +20210,7 @@
       </c>
     </row>
     <row r="60" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="93"/>
+      <c r="B60" s="94"/>
       <c r="C60" s="14" t="s">
         <v>17</v>
       </c>
@@ -20190,7 +20237,7 @@
       </c>
     </row>
     <row r="61" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="98" t="s">
+      <c r="B61" s="92" t="s">
         <v>18</v>
       </c>
       <c r="C61" s="8" t="s">
@@ -20226,7 +20273,7 @@
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B62" s="92"/>
+      <c r="B62" s="93"/>
       <c r="C62" s="9" t="s">
         <v>15</v>
       </c>
@@ -20260,7 +20307,7 @@
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B63" s="92"/>
+      <c r="B63" s="93"/>
       <c r="C63" s="9" t="s">
         <v>16</v>
       </c>
@@ -20294,7 +20341,7 @@
       </c>
     </row>
     <row r="64" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="93"/>
+      <c r="B64" s="94"/>
       <c r="C64" s="14" t="s">
         <v>17</v>
       </c>
@@ -20329,17 +20376,17 @@
     </row>
     <row r="65" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="94" t="s">
+      <c r="B66" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="C66" s="95"/>
-      <c r="D66" s="95"/>
-      <c r="E66" s="95"/>
-      <c r="F66" s="95"/>
-      <c r="G66" s="95"/>
-      <c r="H66" s="95"/>
-      <c r="I66" s="95"/>
-      <c r="J66" s="96"/>
+      <c r="C66" s="96"/>
+      <c r="D66" s="96"/>
+      <c r="E66" s="96"/>
+      <c r="F66" s="96"/>
+      <c r="G66" s="96"/>
+      <c r="H66" s="96"/>
+      <c r="I66" s="96"/>
+      <c r="J66" s="97"/>
     </row>
     <row r="67" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B67" s="26" t="s">
@@ -20371,7 +20418,7 @@
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B68" s="91">
+      <c r="B68" s="98">
         <v>1</v>
       </c>
       <c r="C68" s="8" t="s">
@@ -20400,7 +20447,7 @@
       </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B69" s="92"/>
+      <c r="B69" s="93"/>
       <c r="C69" s="9" t="s">
         <v>15</v>
       </c>
@@ -20427,7 +20474,7 @@
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B70" s="92"/>
+      <c r="B70" s="93"/>
       <c r="C70" s="9" t="s">
         <v>16</v>
       </c>
@@ -20454,7 +20501,7 @@
       </c>
     </row>
     <row r="71" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="97"/>
+      <c r="B71" s="99"/>
       <c r="C71" s="10" t="s">
         <v>17</v>
       </c>
@@ -20481,7 +20528,7 @@
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B72" s="91">
+      <c r="B72" s="98">
         <v>2</v>
       </c>
       <c r="C72" s="8" t="s">
@@ -20510,7 +20557,7 @@
       </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B73" s="92"/>
+      <c r="B73" s="93"/>
       <c r="C73" s="9" t="s">
         <v>15</v>
       </c>
@@ -20537,7 +20584,7 @@
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B74" s="92"/>
+      <c r="B74" s="93"/>
       <c r="C74" s="9" t="s">
         <v>16</v>
       </c>
@@ -20564,7 +20611,7 @@
       </c>
     </row>
     <row r="75" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="97"/>
+      <c r="B75" s="99"/>
       <c r="C75" s="10" t="s">
         <v>17</v>
       </c>
@@ -20591,7 +20638,7 @@
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B76" s="91">
+      <c r="B76" s="98">
         <v>3</v>
       </c>
       <c r="C76" s="8" t="s">
@@ -20620,7 +20667,7 @@
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B77" s="92"/>
+      <c r="B77" s="93"/>
       <c r="C77" s="9" t="s">
         <v>15</v>
       </c>
@@ -20647,7 +20694,7 @@
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B78" s="92"/>
+      <c r="B78" s="93"/>
       <c r="C78" s="9" t="s">
         <v>16</v>
       </c>
@@ -20674,7 +20721,7 @@
       </c>
     </row>
     <row r="79" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="97"/>
+      <c r="B79" s="99"/>
       <c r="C79" s="10" t="s">
         <v>17</v>
       </c>
@@ -20701,7 +20748,7 @@
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B80" s="91">
+      <c r="B80" s="98">
         <v>4</v>
       </c>
       <c r="C80" s="8" t="s">
@@ -20730,7 +20777,7 @@
       </c>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B81" s="92"/>
+      <c r="B81" s="93"/>
       <c r="C81" s="9" t="s">
         <v>15</v>
       </c>
@@ -20757,7 +20804,7 @@
       </c>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B82" s="92"/>
+      <c r="B82" s="93"/>
       <c r="C82" s="9" t="s">
         <v>16</v>
       </c>
@@ -20784,7 +20831,7 @@
       </c>
     </row>
     <row r="83" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="97"/>
+      <c r="B83" s="99"/>
       <c r="C83" s="10" t="s">
         <v>17</v>
       </c>
@@ -20811,7 +20858,7 @@
       </c>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B84" s="91">
+      <c r="B84" s="98">
         <v>5</v>
       </c>
       <c r="C84" s="8" t="s">
@@ -20840,7 +20887,7 @@
       </c>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B85" s="92"/>
+      <c r="B85" s="93"/>
       <c r="C85" s="9" t="s">
         <v>15</v>
       </c>
@@ -20867,7 +20914,7 @@
       </c>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B86" s="92"/>
+      <c r="B86" s="93"/>
       <c r="C86" s="9" t="s">
         <v>16</v>
       </c>
@@ -20894,7 +20941,7 @@
       </c>
     </row>
     <row r="87" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="93"/>
+      <c r="B87" s="94"/>
       <c r="C87" s="14" t="s">
         <v>17</v>
       </c>
@@ -20921,7 +20968,7 @@
       </c>
     </row>
     <row r="88" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="98" t="s">
+      <c r="B88" s="92" t="s">
         <v>18</v>
       </c>
       <c r="C88" s="8" t="s">
@@ -20957,7 +21004,7 @@
       </c>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B89" s="92"/>
+      <c r="B89" s="93"/>
       <c r="C89" s="9" t="s">
         <v>15</v>
       </c>
@@ -20991,7 +21038,7 @@
       </c>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B90" s="92"/>
+      <c r="B90" s="93"/>
       <c r="C90" s="9" t="s">
         <v>16</v>
       </c>
@@ -21025,7 +21072,7 @@
       </c>
     </row>
     <row r="91" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="93"/>
+      <c r="B91" s="94"/>
       <c r="C91" s="14" t="s">
         <v>17</v>
       </c>
@@ -21061,15 +21108,6 @@
     <row r="92" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="B88:B91"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="B66:J66"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="B76:B79"/>
     <mergeCell ref="B53:B56"/>
     <mergeCell ref="B11:J11"/>
     <mergeCell ref="B13:B16"/>
@@ -21082,6 +21120,15 @@
     <mergeCell ref="B41:B44"/>
     <mergeCell ref="B45:B48"/>
     <mergeCell ref="B49:B52"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="B66:J66"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="B76:B79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -21114,14 +21161,14 @@
     <row r="1" spans="6:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="6:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F2" s="55"/>
-      <c r="G2" s="102" t="s">
+      <c r="G2" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="104"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="105"/>
     </row>
     <row r="3" spans="6:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F3" s="56"/>
@@ -21281,27 +21328,27 @@
     <row r="14" spans="6:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="6:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F15" s="36"/>
-      <c r="G15" s="102" t="s">
+      <c r="G15" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="103"/>
-      <c r="I15" s="103"/>
-      <c r="J15" s="103"/>
-      <c r="K15" s="103"/>
-      <c r="L15" s="104"/>
+      <c r="H15" s="104"/>
+      <c r="I15" s="104"/>
+      <c r="J15" s="104"/>
+      <c r="K15" s="104"/>
+      <c r="L15" s="105"/>
     </row>
     <row r="16" spans="6:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F16" s="36"/>
-      <c r="G16" s="99" t="s">
+      <c r="G16" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="H16" s="100"/>
-      <c r="I16" s="101"/>
-      <c r="J16" s="102" t="s">
+      <c r="H16" s="101"/>
+      <c r="I16" s="102"/>
+      <c r="J16" s="103" t="s">
         <v>31</v>
       </c>
-      <c r="K16" s="103"/>
-      <c r="L16" s="104"/>
+      <c r="K16" s="104"/>
+      <c r="L16" s="105"/>
     </row>
     <row r="17" spans="6:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F17" s="36"/>
@@ -21516,15 +21563,15 @@
   <sheetData>
     <row r="5" spans="5:38" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="5:38" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="102" t="s">
+      <c r="E6" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
-      <c r="J6" s="106"/>
-      <c r="K6" s="107"/>
+      <c r="F6" s="107"/>
+      <c r="G6" s="107"/>
+      <c r="H6" s="107"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="108"/>
     </row>
     <row r="7" spans="5:38" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E7" s="71" t="s">
@@ -21548,14 +21595,14 @@
       <c r="K7" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="O7" s="108" t="s">
+      <c r="O7" s="109" t="s">
         <v>27</v>
       </c>
-      <c r="P7" s="109"/>
-      <c r="AB7" s="108" t="s">
+      <c r="P7" s="110"/>
+      <c r="AB7" s="109" t="s">
         <v>65</v>
       </c>
-      <c r="AC7" s="109"/>
+      <c r="AC7" s="110"/>
     </row>
     <row r="8" spans="5:38" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E8" s="61" t="s">
@@ -21602,38 +21649,38 @@
       <c r="K9" s="53">
         <v>2.0348259999999998</v>
       </c>
-      <c r="O9" s="94" t="s">
+      <c r="O9" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="P9" s="96"/>
-      <c r="R9" s="94" t="s">
+      <c r="P9" s="97"/>
+      <c r="R9" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="S9" s="96"/>
-      <c r="U9" s="94" t="s">
+      <c r="S9" s="97"/>
+      <c r="U9" s="95" t="s">
         <v>63</v>
       </c>
-      <c r="V9" s="96"/>
-      <c r="X9" s="94" t="s">
+      <c r="V9" s="97"/>
+      <c r="X9" s="95" t="s">
         <v>64</v>
       </c>
-      <c r="Y9" s="96"/>
-      <c r="AB9" s="94" t="s">
+      <c r="Y9" s="97"/>
+      <c r="AB9" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="AC9" s="96"/>
-      <c r="AE9" s="94" t="s">
+      <c r="AC9" s="97"/>
+      <c r="AE9" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="AF9" s="96"/>
-      <c r="AH9" s="94" t="s">
+      <c r="AF9" s="97"/>
+      <c r="AH9" s="95" t="s">
         <v>63</v>
       </c>
-      <c r="AI9" s="96"/>
-      <c r="AK9" s="94" t="s">
+      <c r="AI9" s="97"/>
+      <c r="AK9" s="95" t="s">
         <v>64</v>
       </c>
-      <c r="AL9" s="96"/>
+      <c r="AL9" s="97"/>
     </row>
     <row r="10" spans="5:38" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E10" s="63" t="s">
@@ -22123,15 +22170,15 @@
       </c>
     </row>
     <row r="17" spans="5:38" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E17" s="102" t="s">
+      <c r="E17" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="106"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="106"/>
-      <c r="J17" s="106"/>
-      <c r="K17" s="107"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="107"/>
+      <c r="H17" s="107"/>
+      <c r="I17" s="107"/>
+      <c r="J17" s="107"/>
+      <c r="K17" s="108"/>
       <c r="O17" s="75">
         <v>2.0833333333333333E-3</v>
       </c>
@@ -22882,15 +22929,15 @@
       </c>
     </row>
     <row r="28" spans="5:38" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E28" s="102" t="s">
+      <c r="E28" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="F28" s="106"/>
-      <c r="G28" s="106"/>
-      <c r="H28" s="106"/>
-      <c r="I28" s="106"/>
-      <c r="J28" s="106"/>
-      <c r="K28" s="107"/>
+      <c r="F28" s="107"/>
+      <c r="G28" s="107"/>
+      <c r="H28" s="107"/>
+      <c r="I28" s="107"/>
+      <c r="J28" s="107"/>
+      <c r="K28" s="108"/>
       <c r="O28" s="74">
         <v>5.9027777777777802E-3</v>
       </c>
@@ -23304,15 +23351,15 @@
     </row>
     <row r="38" spans="5:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="5:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E39" s="102" t="s">
+      <c r="E39" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="F39" s="106"/>
-      <c r="G39" s="106"/>
-      <c r="H39" s="106"/>
-      <c r="I39" s="106"/>
-      <c r="J39" s="106"/>
-      <c r="K39" s="107"/>
+      <c r="F39" s="107"/>
+      <c r="G39" s="107"/>
+      <c r="H39" s="107"/>
+      <c r="I39" s="107"/>
+      <c r="J39" s="107"/>
+      <c r="K39" s="108"/>
     </row>
     <row r="40" spans="5:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E40" s="71" t="s">
@@ -23534,15 +23581,15 @@
     </row>
     <row r="49" spans="5:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="50" spans="5:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E50" s="102" t="s">
+      <c r="E50" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="F50" s="106"/>
-      <c r="G50" s="106"/>
-      <c r="H50" s="106"/>
-      <c r="I50" s="106"/>
-      <c r="J50" s="106"/>
-      <c r="K50" s="107"/>
+      <c r="F50" s="107"/>
+      <c r="G50" s="107"/>
+      <c r="H50" s="107"/>
+      <c r="I50" s="107"/>
+      <c r="J50" s="107"/>
+      <c r="K50" s="108"/>
     </row>
     <row r="51" spans="5:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E51" s="71" t="s">
@@ -23674,7 +23721,7 @@
       <c r="I58" s="77"/>
       <c r="J58" s="77"/>
       <c r="K58" s="77"/>
-      <c r="P58" s="81"/>
+      <c r="P58" s="80"/>
     </row>
     <row r="59" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E59" s="77"/>
@@ -23684,7 +23731,7 @@
       <c r="I59" s="77"/>
       <c r="J59" s="77"/>
       <c r="K59" s="77"/>
-      <c r="P59" s="81"/>
+      <c r="P59" s="80"/>
     </row>
     <row r="60" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E60" s="77"/>
@@ -23706,21 +23753,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="E17:K17"/>
+    <mergeCell ref="E50:K50"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="X9:Y9"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="AB9:AC9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="O7:P7"/>
     <mergeCell ref="AE9:AF9"/>
     <mergeCell ref="AH9:AI9"/>
     <mergeCell ref="AK9:AL9"/>
     <mergeCell ref="E28:K28"/>
     <mergeCell ref="E39:K39"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="AB9:AC9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="E6:K6"/>
-    <mergeCell ref="E17:K17"/>
-    <mergeCell ref="E50:K50"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="X9:Y9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -23731,8 +23778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED086EA8-21A2-AA4E-8784-EC5D248DD200}">
   <dimension ref="C3:S53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="F38" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23750,27 +23797,27 @@
   <sheetData>
     <row r="3" spans="3:18" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="3:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="102" t="s">
+      <c r="C4" s="103" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="107"/>
-      <c r="K4" s="94" t="s">
+      <c r="D4" s="107"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="107"/>
+      <c r="G4" s="107"/>
+      <c r="H4" s="107"/>
+      <c r="I4" s="108"/>
+      <c r="K4" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="96"/>
-      <c r="N4" s="94" t="s">
+      <c r="L4" s="97"/>
+      <c r="N4" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="O4" s="96"/>
-      <c r="Q4" s="94" t="s">
+      <c r="O4" s="97"/>
+      <c r="Q4" s="95" t="s">
         <v>74</v>
       </c>
-      <c r="R4" s="96"/>
+      <c r="R4" s="97"/>
     </row>
     <row r="5" spans="3:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="42" t="s">
@@ -23794,22 +23841,22 @@
       <c r="I5" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="89" t="s">
+      <c r="K5" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="90" t="s">
+      <c r="L5" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="N5" s="89" t="s">
+      <c r="N5" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="90" t="s">
+      <c r="O5" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="Q5" s="89" t="s">
+      <c r="Q5" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="R5" s="90" t="s">
+      <c r="R5" s="89" t="s">
         <v>26</v>
       </c>
     </row>
@@ -23896,7 +23943,7 @@
       </c>
     </row>
     <row r="8" spans="3:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="81" t="s">
         <v>74</v>
       </c>
       <c r="D8" s="47">
@@ -23938,12 +23985,12 @@
     </row>
     <row r="9" spans="3:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="76"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="83"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
       <c r="K9" s="74">
         <v>1.0416666666666667E-3</v>
       </c>
@@ -23965,12 +24012,12 @@
     </row>
     <row r="10" spans="3:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C10" s="77"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
       <c r="K10" s="74">
         <v>1.3888888888888889E-3</v>
       </c>
@@ -23992,12 +24039,12 @@
     </row>
     <row r="11" spans="3:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C11" s="77"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="84"/>
-      <c r="I11" s="84"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="83"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="83"/>
+      <c r="I11" s="83"/>
       <c r="K11" s="74">
         <v>1.736111111111111E-3</v>
       </c>
@@ -24072,13 +24119,13 @@
       </c>
     </row>
     <row r="14" spans="3:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="81"/>
-      <c r="D14" s="81"/>
-      <c r="E14" s="81"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="81"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
       <c r="K14" s="74">
         <v>2.7777777777777801E-3</v>
       </c>
@@ -24125,13 +24172,13 @@
       <c r="L16" s="35">
         <v>23</v>
       </c>
-      <c r="N16" s="85">
+      <c r="N16" s="84">
         <v>3.4722222222222199E-3</v>
       </c>
       <c r="O16" s="11">
         <v>16</v>
       </c>
-      <c r="Q16" s="85">
+      <c r="Q16" s="84">
         <v>3.4722222222222199E-3</v>
       </c>
       <c r="R16" s="11">
@@ -24139,117 +24186,117 @@
       </c>
     </row>
     <row r="17" spans="11:18" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="K17" s="88"/>
-      <c r="L17" s="81"/>
-      <c r="N17" s="86"/>
-      <c r="O17" s="87"/>
-      <c r="Q17" s="86"/>
-      <c r="R17" s="87"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="80"/>
+      <c r="N17" s="85"/>
+      <c r="O17" s="86"/>
+      <c r="Q17" s="85"/>
+      <c r="R17" s="86"/>
     </row>
     <row r="18" spans="11:18" x14ac:dyDescent="0.2">
-      <c r="K18" s="88"/>
-      <c r="L18" s="81"/>
-      <c r="N18" s="88"/>
-      <c r="O18" s="81"/>
-      <c r="Q18" s="88"/>
-      <c r="R18" s="81"/>
+      <c r="K18" s="87"/>
+      <c r="L18" s="80"/>
+      <c r="N18" s="87"/>
+      <c r="O18" s="80"/>
+      <c r="Q18" s="87"/>
+      <c r="R18" s="80"/>
     </row>
     <row r="19" spans="11:18" x14ac:dyDescent="0.2">
-      <c r="K19" s="88"/>
-      <c r="L19" s="81"/>
-      <c r="N19" s="88"/>
-      <c r="O19" s="81"/>
-      <c r="Q19" s="88"/>
-      <c r="R19" s="81"/>
+      <c r="K19" s="87"/>
+      <c r="L19" s="80"/>
+      <c r="N19" s="87"/>
+      <c r="O19" s="80"/>
+      <c r="Q19" s="87"/>
+      <c r="R19" s="80"/>
     </row>
     <row r="20" spans="11:18" x14ac:dyDescent="0.2">
-      <c r="K20" s="88"/>
-      <c r="L20" s="81"/>
-      <c r="N20" s="88"/>
-      <c r="O20" s="81"/>
-      <c r="Q20" s="88"/>
-      <c r="R20" s="81"/>
+      <c r="K20" s="87"/>
+      <c r="L20" s="80"/>
+      <c r="N20" s="87"/>
+      <c r="O20" s="80"/>
+      <c r="Q20" s="87"/>
+      <c r="R20" s="80"/>
     </row>
     <row r="21" spans="11:18" x14ac:dyDescent="0.2">
-      <c r="K21" s="88"/>
-      <c r="L21" s="81"/>
-      <c r="N21" s="88"/>
-      <c r="O21" s="81"/>
-      <c r="Q21" s="88"/>
-      <c r="R21" s="81"/>
+      <c r="K21" s="87"/>
+      <c r="L21" s="80"/>
+      <c r="N21" s="87"/>
+      <c r="O21" s="80"/>
+      <c r="Q21" s="87"/>
+      <c r="R21" s="80"/>
     </row>
     <row r="22" spans="11:18" x14ac:dyDescent="0.2">
-      <c r="K22" s="88"/>
-      <c r="L22" s="81"/>
-      <c r="N22" s="88"/>
-      <c r="O22" s="81"/>
-      <c r="Q22" s="88"/>
-      <c r="R22" s="81"/>
+      <c r="K22" s="87"/>
+      <c r="L22" s="80"/>
+      <c r="N22" s="87"/>
+      <c r="O22" s="80"/>
+      <c r="Q22" s="87"/>
+      <c r="R22" s="80"/>
     </row>
     <row r="23" spans="11:18" x14ac:dyDescent="0.2">
-      <c r="K23" s="88"/>
-      <c r="L23" s="81"/>
-      <c r="N23" s="88"/>
-      <c r="O23" s="81"/>
-      <c r="Q23" s="88"/>
-      <c r="R23" s="81"/>
+      <c r="K23" s="87"/>
+      <c r="L23" s="80"/>
+      <c r="N23" s="87"/>
+      <c r="O23" s="80"/>
+      <c r="Q23" s="87"/>
+      <c r="R23" s="80"/>
     </row>
     <row r="24" spans="11:18" x14ac:dyDescent="0.2">
-      <c r="K24" s="88"/>
-      <c r="L24" s="81"/>
-      <c r="N24" s="88"/>
-      <c r="O24" s="81"/>
-      <c r="Q24" s="88"/>
-      <c r="R24" s="81"/>
+      <c r="K24" s="87"/>
+      <c r="L24" s="80"/>
+      <c r="N24" s="87"/>
+      <c r="O24" s="80"/>
+      <c r="Q24" s="87"/>
+      <c r="R24" s="80"/>
     </row>
     <row r="25" spans="11:18" x14ac:dyDescent="0.2">
-      <c r="K25" s="88"/>
-      <c r="L25" s="81"/>
-      <c r="N25" s="88"/>
-      <c r="O25" s="81"/>
-      <c r="Q25" s="88"/>
-      <c r="R25" s="81"/>
+      <c r="K25" s="87"/>
+      <c r="L25" s="80"/>
+      <c r="N25" s="87"/>
+      <c r="O25" s="80"/>
+      <c r="Q25" s="87"/>
+      <c r="R25" s="80"/>
     </row>
     <row r="26" spans="11:18" x14ac:dyDescent="0.2">
-      <c r="K26" s="88"/>
-      <c r="L26" s="81"/>
-      <c r="N26" s="88"/>
-      <c r="O26" s="81"/>
-      <c r="Q26" s="88"/>
-      <c r="R26" s="81"/>
+      <c r="K26" s="87"/>
+      <c r="L26" s="80"/>
+      <c r="N26" s="87"/>
+      <c r="O26" s="80"/>
+      <c r="Q26" s="87"/>
+      <c r="R26" s="80"/>
     </row>
     <row r="39" spans="3:19" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="3:19" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L40" s="94" t="s">
+      <c r="L40" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="M40" s="96"/>
-      <c r="O40" s="94" t="s">
+      <c r="M40" s="97"/>
+      <c r="O40" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="P40" s="96"/>
-      <c r="R40" s="94" t="s">
+      <c r="P40" s="97"/>
+      <c r="R40" s="95" t="s">
         <v>74</v>
       </c>
-      <c r="S40" s="96"/>
+      <c r="S40" s="97"/>
     </row>
     <row r="41" spans="3:19" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L41" s="89" t="s">
+      <c r="L41" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="M41" s="90" t="s">
+      <c r="M41" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="O41" s="89" t="s">
+      <c r="O41" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="P41" s="90" t="s">
+      <c r="P41" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="R41" s="89" t="s">
+      <c r="R41" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="S41" s="90" t="s">
+      <c r="S41" s="89" t="s">
         <v>26</v>
       </c>
     </row>
@@ -24258,7 +24305,7 @@
         <v>0</v>
       </c>
       <c r="M42" s="34">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="O42" s="74">
         <v>0</v>
@@ -24270,7 +24317,7 @@
         <v>0</v>
       </c>
       <c r="S42" s="34">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="3:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -24278,7 +24325,7 @@
         <v>3.4722222222222224E-4</v>
       </c>
       <c r="M43" s="34">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="O43" s="74">
         <v>3.4722222222222224E-4</v>
@@ -24298,19 +24345,19 @@
         <v>6.9444444444444447E-4</v>
       </c>
       <c r="M44" s="34">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="O44" s="74">
         <v>6.9444444444444447E-4</v>
       </c>
       <c r="P44" s="34">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R44" s="74">
         <v>6.9444444444444447E-4</v>
       </c>
       <c r="S44" s="34">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="3:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -24318,13 +24365,13 @@
         <v>1.0416666666666667E-3</v>
       </c>
       <c r="M45" s="34">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="O45" s="74">
         <v>1.0416666666666667E-3</v>
       </c>
       <c r="P45" s="34">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R45" s="74">
         <v>1.0416666666666667E-3</v>
@@ -24338,13 +24385,13 @@
         <v>1.3888888888888889E-3</v>
       </c>
       <c r="M46" s="34">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O46" s="74">
         <v>1.3888888888888889E-3</v>
       </c>
       <c r="P46" s="34">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R46" s="74">
         <v>1.3888888888888889E-3</v>
@@ -24354,32 +24401,32 @@
       </c>
     </row>
     <row r="47" spans="3:19" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="102" t="s">
+      <c r="C47" s="103" t="s">
         <v>77</v>
       </c>
-      <c r="D47" s="106"/>
-      <c r="E47" s="106"/>
-      <c r="F47" s="106"/>
-      <c r="G47" s="106"/>
-      <c r="H47" s="106"/>
-      <c r="I47" s="107"/>
+      <c r="D47" s="107"/>
+      <c r="E47" s="107"/>
+      <c r="F47" s="107"/>
+      <c r="G47" s="107"/>
+      <c r="H47" s="107"/>
+      <c r="I47" s="108"/>
       <c r="L47" s="74">
         <v>1.736111111111111E-3</v>
       </c>
       <c r="M47" s="34">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="O47" s="74">
         <v>1.736111111111111E-3</v>
       </c>
       <c r="P47" s="34">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="R47" s="74">
         <v>1.736111111111111E-3</v>
       </c>
       <c r="S47" s="34">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="3:19" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -24389,13 +24436,13 @@
       <c r="D48" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="E48" s="80" t="s">
+      <c r="E48" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="80" t="s">
+      <c r="F48" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="G48" s="80" t="s">
+      <c r="G48" s="90" t="s">
         <v>42</v>
       </c>
       <c r="H48" s="59">
@@ -24408,19 +24455,19 @@
         <v>2.0833333333333333E-3</v>
       </c>
       <c r="M48" s="35">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O48" s="75">
         <v>2.0833333333333333E-3</v>
       </c>
       <c r="P48" s="35">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R48" s="75">
         <v>2.0833333333333333E-3</v>
       </c>
       <c r="S48" s="35">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="3:19" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -24431,29 +24478,31 @@
         <v>5</v>
       </c>
       <c r="E49" s="44">
-        <v>4484</v>
+        <v>5718</v>
       </c>
       <c r="F49" s="44">
-        <v>67</v>
-      </c>
-      <c r="G49" s="110">
-        <v>24</v>
+        <v>52</v>
+      </c>
+      <c r="G49" s="91">
+        <v>20</v>
       </c>
       <c r="H49" s="62">
-        <v>81</v>
-      </c>
-      <c r="I49" s="53"/>
+        <v>68</v>
+      </c>
+      <c r="I49" s="53" t="s">
+        <v>78</v>
+      </c>
       <c r="L49" s="74">
         <v>2.4305555555555599E-3</v>
       </c>
       <c r="M49" s="34">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="O49" s="74">
         <v>2.4305555555555599E-3</v>
       </c>
       <c r="P49" s="34">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="R49" s="74">
         <v>2.4305555555555599E-3</v>
@@ -24470,99 +24519,104 @@
         <v>5</v>
       </c>
       <c r="E50" s="44">
-        <v>3571</v>
+        <v>4238</v>
       </c>
       <c r="F50" s="44">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="G50" s="44">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H50" s="62">
-        <v>130</v>
-      </c>
-      <c r="I50" s="53"/>
+        <v>117</v>
+      </c>
+      <c r="I50" s="53" t="s">
+        <v>79</v>
+      </c>
       <c r="L50" s="74">
         <v>2.7777777777777801E-3</v>
       </c>
       <c r="M50" s="34">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="O50" s="74">
         <v>2.7777777777777801E-3</v>
       </c>
       <c r="P50" s="34">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="R50" s="74">
         <v>2.7777777777777801E-3</v>
       </c>
       <c r="S50" s="34">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="3:19" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C51" s="82" t="s">
+      <c r="C51" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="D51" s="47">
+      <c r="D51" s="111">
         <v>5</v>
       </c>
-      <c r="E51" s="48">
-        <v>2655</v>
-      </c>
-      <c r="F51" s="48">
-        <v>113</v>
-      </c>
-      <c r="G51" s="48">
-        <v>33</v>
-      </c>
-      <c r="H51" s="66">
-        <v>163</v>
-      </c>
-      <c r="I51" s="67"/>
+      <c r="E51" s="112">
+        <v>3016</v>
+      </c>
+      <c r="F51" s="112">
+        <v>99</v>
+      </c>
+      <c r="G51" s="112">
+        <v>30</v>
+      </c>
+      <c r="H51" s="113">
+        <v>150</v>
+      </c>
+      <c r="I51" s="114" t="s">
+        <v>80</v>
+      </c>
       <c r="L51" s="74">
         <v>3.1250000000000002E-3</v>
       </c>
       <c r="M51" s="34">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="O51" s="74">
         <v>3.1250000000000002E-3</v>
       </c>
       <c r="P51" s="34">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="R51" s="74">
         <v>3.1250000000000002E-3</v>
       </c>
       <c r="S51" s="34">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="3:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="3:19" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L52" s="75">
         <v>3.472222222222222E-3</v>
       </c>
       <c r="M52" s="35">
-        <v>15</v>
-      </c>
-      <c r="O52" s="85">
+        <v>22</v>
+      </c>
+      <c r="O52" s="75">
         <v>3.4722222222222199E-3</v>
       </c>
-      <c r="P52" s="11">
-        <v>13</v>
-      </c>
-      <c r="R52" s="85">
+      <c r="P52" s="35">
+        <v>14</v>
+      </c>
+      <c r="R52" s="75">
         <v>3.4722222222222199E-3</v>
       </c>
-      <c r="S52" s="11">
+      <c r="S52" s="35">
         <v>9</v>
       </c>
     </row>
     <row r="53" spans="3:19" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C47:I47"/>
     <mergeCell ref="L40:M40"/>
     <mergeCell ref="O40:P40"/>
     <mergeCell ref="R40:S40"/>
@@ -24570,7 +24624,6 @@
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="N4:O4"/>
     <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="C47:I47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added redis cluster memory usage section
</commit_message>
<xml_diff>
--- a/thesis-tests.xlsx
+++ b/thesis-tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguelanciaes/Desktop/thesis/novathesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C827F164-F1EA-7F4B-90B3-8A5978CC22C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F368F1E-A69E-F44F-9D4D-FB8B8CEF1C47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="2" activeTab="7" xr2:uid="{6308EBAC-DE62-D645-97F4-0D2E9D77B78B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="2" activeTab="8" xr2:uid="{6308EBAC-DE62-D645-97F4-0D2E9D77B78B}"/>
   </bookViews>
   <sheets>
     <sheet name="External Redis-Benchmarks" sheetId="2" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Cluster Redis" sheetId="7" r:id="rId6"/>
     <sheet name="Memory &amp; CPU" sheetId="8" r:id="rId7"/>
     <sheet name="Performance over Size" sheetId="9" r:id="rId8"/>
+    <sheet name="Cluster Nodes Memory" sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Memory &amp; CPU'!$AN$125:$AU$521</definedName>
@@ -141,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2761" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2768" uniqueCount="835">
   <si>
     <t>Test Configurations</t>
   </si>
@@ -2634,6 +2635,18 @@
   </si>
   <si>
     <t>Average Latency</t>
+  </si>
+  <si>
+    <t>Standalone Memory</t>
+  </si>
+  <si>
+    <t>Masters</t>
+  </si>
+  <si>
+    <t>Total Memory (Masters)</t>
+  </si>
+  <si>
+    <t>Slaves</t>
   </si>
 </sst>
 </file>
@@ -3526,7 +3539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="205">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -3866,7 +3879,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="45" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3884,10 +3897,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3919,15 +3932,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3939,6 +3943,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3965,6 +3978,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -36127,23 +36149,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_5" connectionId="4" xr16:uid="{F7C01357-A0B7-9C46-A14F-E3A5D11E2DD6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_1" connectionId="5" xr16:uid="{83893D2E-64E6-4141-91BF-17E4FBF6D821}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_2" connectionId="1" xr16:uid="{EE16474F-CCD2-364B-A607-51BAF623E71C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_3" connectionId="2" xr16:uid="{493998F8-C237-CC45-95DE-DE52776EC4BA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_6" connectionId="6" xr16:uid="{F0609839-D860-594D-A6DC-121FFC03226C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tests_5" connectionId="4" xr16:uid="{F7C01357-A0B7-9C46-A14F-E3A5D11E2DD6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36546,7 +36568,7 @@
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="169">
+      <c r="B13" s="163">
         <v>1</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -36629,7 +36651,7 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="170"/>
+      <c r="B16" s="169"/>
       <c r="C16" s="10" t="s">
         <v>17</v>
       </c>
@@ -36656,7 +36678,7 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="169">
+      <c r="B17" s="163">
         <v>2</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -36739,7 +36761,7 @@
       </c>
     </row>
     <row r="20" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="170"/>
+      <c r="B20" s="169"/>
       <c r="C20" s="10" t="s">
         <v>17</v>
       </c>
@@ -36766,7 +36788,7 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="169">
+      <c r="B21" s="163">
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -36849,7 +36871,7 @@
       </c>
     </row>
     <row r="24" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="170"/>
+      <c r="B24" s="169"/>
       <c r="C24" s="10" t="s">
         <v>17</v>
       </c>
@@ -36876,7 +36898,7 @@
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="169">
+      <c r="B25" s="163">
         <v>4</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -36959,7 +36981,7 @@
       </c>
     </row>
     <row r="28" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="170"/>
+      <c r="B28" s="169"/>
       <c r="C28" s="10" t="s">
         <v>17</v>
       </c>
@@ -36986,7 +37008,7 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="169">
+      <c r="B29" s="163">
         <v>5</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -37096,7 +37118,7 @@
       </c>
     </row>
     <row r="33" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="163" t="s">
+      <c r="B33" s="170" t="s">
         <v>18</v>
       </c>
       <c r="C33" s="16" t="s">
@@ -37278,7 +37300,7 @@
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="169">
+      <c r="B41" s="163">
         <v>1</v>
       </c>
       <c r="C41" s="8" t="s">
@@ -37361,7 +37383,7 @@
       </c>
     </row>
     <row r="44" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="170"/>
+      <c r="B44" s="169"/>
       <c r="C44" s="10" t="s">
         <v>17</v>
       </c>
@@ -37388,7 +37410,7 @@
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B45" s="169">
+      <c r="B45" s="163">
         <v>2</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -37471,7 +37493,7 @@
       </c>
     </row>
     <row r="48" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="170"/>
+      <c r="B48" s="169"/>
       <c r="C48" s="10" t="s">
         <v>17</v>
       </c>
@@ -37498,7 +37520,7 @@
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B49" s="169">
+      <c r="B49" s="163">
         <v>3</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -37581,7 +37603,7 @@
       </c>
     </row>
     <row r="52" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="170"/>
+      <c r="B52" s="169"/>
       <c r="C52" s="10" t="s">
         <v>17</v>
       </c>
@@ -37608,7 +37630,7 @@
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B53" s="169">
+      <c r="B53" s="163">
         <v>4</v>
       </c>
       <c r="C53" s="8" t="s">
@@ -37691,7 +37713,7 @@
       </c>
     </row>
     <row r="56" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="170"/>
+      <c r="B56" s="169"/>
       <c r="C56" s="10" t="s">
         <v>17</v>
       </c>
@@ -37718,7 +37740,7 @@
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" s="169">
+      <c r="B57" s="163">
         <v>5</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -37828,7 +37850,7 @@
       </c>
     </row>
     <row r="61" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="163" t="s">
+      <c r="B61" s="170" t="s">
         <v>18</v>
       </c>
       <c r="C61" s="16" t="s">
@@ -38009,7 +38031,7 @@
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B68" s="169">
+      <c r="B68" s="163">
         <v>1</v>
       </c>
       <c r="C68" s="8" t="s">
@@ -38092,7 +38114,7 @@
       </c>
     </row>
     <row r="71" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="170"/>
+      <c r="B71" s="169"/>
       <c r="C71" s="10" t="s">
         <v>17</v>
       </c>
@@ -38119,7 +38141,7 @@
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B72" s="169">
+      <c r="B72" s="163">
         <v>2</v>
       </c>
       <c r="C72" s="8" t="s">
@@ -38202,7 +38224,7 @@
       </c>
     </row>
     <row r="75" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="170"/>
+      <c r="B75" s="169"/>
       <c r="C75" s="10" t="s">
         <v>17</v>
       </c>
@@ -38229,7 +38251,7 @@
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B76" s="169">
+      <c r="B76" s="163">
         <v>3</v>
       </c>
       <c r="C76" s="8" t="s">
@@ -38312,7 +38334,7 @@
       </c>
     </row>
     <row r="79" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="170"/>
+      <c r="B79" s="169"/>
       <c r="C79" s="10" t="s">
         <v>17</v>
       </c>
@@ -38339,7 +38361,7 @@
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B80" s="169">
+      <c r="B80" s="163">
         <v>4</v>
       </c>
       <c r="C80" s="8" t="s">
@@ -38422,7 +38444,7 @@
       </c>
     </row>
     <row r="83" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="170"/>
+      <c r="B83" s="169"/>
       <c r="C83" s="10" t="s">
         <v>17</v>
       </c>
@@ -38449,7 +38471,7 @@
       </c>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B84" s="169">
+      <c r="B84" s="163">
         <v>5</v>
       </c>
       <c r="C84" s="8" t="s">
@@ -38559,7 +38581,7 @@
       </c>
     </row>
     <row r="88" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="163" t="s">
+      <c r="B88" s="170" t="s">
         <v>18</v>
       </c>
       <c r="C88" s="16" t="s">
@@ -38699,12 +38721,6 @@
     <row r="92" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="B11:J11"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B25:B28"/>
     <mergeCell ref="B61:B64"/>
     <mergeCell ref="B33:B36"/>
     <mergeCell ref="B88:B91"/>
@@ -38720,6 +38736,12 @@
     <mergeCell ref="B49:B52"/>
     <mergeCell ref="B53:B56"/>
     <mergeCell ref="B57:B60"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B25:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -38831,7 +38853,7 @@
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="169">
+      <c r="B13" s="163">
         <v>1</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -38914,7 +38936,7 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="170"/>
+      <c r="B16" s="169"/>
       <c r="C16" s="10" t="s">
         <v>17</v>
       </c>
@@ -38941,7 +38963,7 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="169">
+      <c r="B17" s="163">
         <v>2</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -39024,7 +39046,7 @@
       </c>
     </row>
     <row r="20" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="170"/>
+      <c r="B20" s="169"/>
       <c r="C20" s="10" t="s">
         <v>17</v>
       </c>
@@ -39051,7 +39073,7 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="169">
+      <c r="B21" s="163">
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -39134,7 +39156,7 @@
       </c>
     </row>
     <row r="24" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="170"/>
+      <c r="B24" s="169"/>
       <c r="C24" s="10" t="s">
         <v>17</v>
       </c>
@@ -39161,7 +39183,7 @@
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="169">
+      <c r="B25" s="163">
         <v>4</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -39244,7 +39266,7 @@
       </c>
     </row>
     <row r="28" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="170"/>
+      <c r="B28" s="169"/>
       <c r="C28" s="10" t="s">
         <v>17</v>
       </c>
@@ -39271,7 +39293,7 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="169">
+      <c r="B29" s="163">
         <v>5</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -39381,7 +39403,7 @@
       </c>
     </row>
     <row r="33" spans="2:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="163" t="s">
+      <c r="B33" s="170" t="s">
         <v>18</v>
       </c>
       <c r="C33" s="8" t="s">
@@ -39563,7 +39585,7 @@
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="169">
+      <c r="B41" s="163">
         <v>1</v>
       </c>
       <c r="C41" s="8" t="s">
@@ -39646,7 +39668,7 @@
       </c>
     </row>
     <row r="44" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="170"/>
+      <c r="B44" s="169"/>
       <c r="C44" s="10" t="s">
         <v>17</v>
       </c>
@@ -39673,7 +39695,7 @@
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B45" s="169">
+      <c r="B45" s="163">
         <v>2</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -39756,7 +39778,7 @@
       </c>
     </row>
     <row r="48" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="170"/>
+      <c r="B48" s="169"/>
       <c r="C48" s="10" t="s">
         <v>17</v>
       </c>
@@ -39783,7 +39805,7 @@
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B49" s="169">
+      <c r="B49" s="163">
         <v>3</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -39866,7 +39888,7 @@
       </c>
     </row>
     <row r="52" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="170"/>
+      <c r="B52" s="169"/>
       <c r="C52" s="10" t="s">
         <v>17</v>
       </c>
@@ -39893,7 +39915,7 @@
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B53" s="169">
+      <c r="B53" s="163">
         <v>4</v>
       </c>
       <c r="C53" s="8" t="s">
@@ -39976,7 +39998,7 @@
       </c>
     </row>
     <row r="56" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="170"/>
+      <c r="B56" s="169"/>
       <c r="C56" s="10" t="s">
         <v>17</v>
       </c>
@@ -40003,7 +40025,7 @@
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" s="169">
+      <c r="B57" s="163">
         <v>5</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -40113,7 +40135,7 @@
       </c>
     </row>
     <row r="61" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="163" t="s">
+      <c r="B61" s="170" t="s">
         <v>18</v>
       </c>
       <c r="C61" s="8" t="s">
@@ -40294,7 +40316,7 @@
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B68" s="169">
+      <c r="B68" s="163">
         <v>1</v>
       </c>
       <c r="C68" s="8" t="s">
@@ -40377,7 +40399,7 @@
       </c>
     </row>
     <row r="71" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="170"/>
+      <c r="B71" s="169"/>
       <c r="C71" s="10" t="s">
         <v>17</v>
       </c>
@@ -40404,7 +40426,7 @@
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B72" s="169">
+      <c r="B72" s="163">
         <v>2</v>
       </c>
       <c r="C72" s="8" t="s">
@@ -40487,7 +40509,7 @@
       </c>
     </row>
     <row r="75" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="170"/>
+      <c r="B75" s="169"/>
       <c r="C75" s="10" t="s">
         <v>17</v>
       </c>
@@ -40514,7 +40536,7 @@
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B76" s="169">
+      <c r="B76" s="163">
         <v>3</v>
       </c>
       <c r="C76" s="8" t="s">
@@ -40597,7 +40619,7 @@
       </c>
     </row>
     <row r="79" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="170"/>
+      <c r="B79" s="169"/>
       <c r="C79" s="10" t="s">
         <v>17</v>
       </c>
@@ -40624,7 +40646,7 @@
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B80" s="169">
+      <c r="B80" s="163">
         <v>4</v>
       </c>
       <c r="C80" s="8" t="s">
@@ -40707,7 +40729,7 @@
       </c>
     </row>
     <row r="83" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="170"/>
+      <c r="B83" s="169"/>
       <c r="C83" s="10" t="s">
         <v>17</v>
       </c>
@@ -40734,7 +40756,7 @@
       </c>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B84" s="169">
+      <c r="B84" s="163">
         <v>5</v>
       </c>
       <c r="C84" s="8" t="s">
@@ -40844,7 +40866,7 @@
       </c>
     </row>
     <row r="88" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="163" t="s">
+      <c r="B88" s="170" t="s">
         <v>18</v>
       </c>
       <c r="C88" s="8" t="s">
@@ -40984,6 +41006,15 @@
     <row r="92" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="B66:J66"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="B76:B79"/>
     <mergeCell ref="B53:B56"/>
     <mergeCell ref="B11:J11"/>
     <mergeCell ref="B13:B16"/>
@@ -40996,15 +41027,6 @@
     <mergeCell ref="B41:B44"/>
     <mergeCell ref="B45:B48"/>
     <mergeCell ref="B49:B52"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="B88:B91"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="B66:J66"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="B76:B79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -44555,21 +44577,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="AH9:AI9"/>
+    <mergeCell ref="AK9:AL9"/>
+    <mergeCell ref="E28:K28"/>
+    <mergeCell ref="E39:K39"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="AB9:AC9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="O7:P7"/>
     <mergeCell ref="E6:K6"/>
     <mergeCell ref="E17:K17"/>
     <mergeCell ref="E50:K50"/>
     <mergeCell ref="U9:V9"/>
     <mergeCell ref="X9:Y9"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="AB9:AC9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="AH9:AI9"/>
-    <mergeCell ref="AK9:AL9"/>
-    <mergeCell ref="E28:K28"/>
-    <mergeCell ref="E39:K39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -44600,7 +44622,7 @@
   <sheetData>
     <row r="5" spans="3:29" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="3:29" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M6" s="184" t="s">
+      <c r="M6" s="188" t="s">
         <v>27</v>
       </c>
       <c r="N6" s="167"/>
@@ -44610,7 +44632,7 @@
       <c r="R6" s="178"/>
       <c r="S6" s="178"/>
       <c r="T6" s="179"/>
-      <c r="V6" s="184" t="s">
+      <c r="V6" s="188" t="s">
         <v>62</v>
       </c>
       <c r="W6" s="167"/>
@@ -44622,43 +44644,43 @@
       <c r="AC6" s="179"/>
     </row>
     <row r="7" spans="3:29" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="185" t="s">
+      <c r="C7" s="182" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="186"/>
-      <c r="E7" s="186"/>
-      <c r="F7" s="186"/>
-      <c r="G7" s="186"/>
-      <c r="H7" s="186"/>
-      <c r="I7" s="187"/>
-      <c r="M7" s="182" t="s">
+      <c r="D7" s="183"/>
+      <c r="E7" s="183"/>
+      <c r="F7" s="183"/>
+      <c r="G7" s="183"/>
+      <c r="H7" s="183"/>
+      <c r="I7" s="184"/>
+      <c r="M7" s="186" t="s">
         <v>58</v>
       </c>
-      <c r="N7" s="183"/>
+      <c r="N7" s="187"/>
       <c r="O7" s="80"/>
-      <c r="P7" s="182" t="s">
+      <c r="P7" s="186" t="s">
         <v>59</v>
       </c>
-      <c r="Q7" s="183"/>
+      <c r="Q7" s="187"/>
       <c r="R7" s="80"/>
-      <c r="S7" s="182" t="s">
+      <c r="S7" s="186" t="s">
         <v>61</v>
       </c>
-      <c r="T7" s="183"/>
-      <c r="V7" s="182" t="s">
+      <c r="T7" s="187"/>
+      <c r="V7" s="186" t="s">
         <v>58</v>
       </c>
-      <c r="W7" s="183"/>
+      <c r="W7" s="187"/>
       <c r="X7" s="80"/>
-      <c r="Y7" s="182" t="s">
+      <c r="Y7" s="186" t="s">
         <v>59</v>
       </c>
-      <c r="Z7" s="183"/>
+      <c r="Z7" s="187"/>
       <c r="AA7" s="80"/>
-      <c r="AB7" s="182" t="s">
+      <c r="AB7" s="186" t="s">
         <v>61</v>
       </c>
-      <c r="AC7" s="183"/>
+      <c r="AC7" s="187"/>
     </row>
     <row r="8" spans="3:29" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="97" t="s">
@@ -45281,15 +45303,15 @@
       </c>
     </row>
     <row r="18" spans="3:29" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="185" t="s">
+      <c r="C18" s="182" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="186"/>
-      <c r="E18" s="186"/>
-      <c r="F18" s="186"/>
-      <c r="G18" s="186"/>
-      <c r="H18" s="186"/>
-      <c r="I18" s="187"/>
+      <c r="D18" s="183"/>
+      <c r="E18" s="183"/>
+      <c r="F18" s="183"/>
+      <c r="G18" s="183"/>
+      <c r="H18" s="183"/>
+      <c r="I18" s="184"/>
       <c r="M18" s="74">
         <v>3.1250000000000002E-3</v>
       </c>
@@ -45956,7 +45978,7 @@
       </c>
     </row>
     <row r="29" spans="3:29" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="185" t="s">
+      <c r="C29" s="182" t="s">
         <v>55</v>
       </c>
       <c r="D29" s="176"/>
@@ -45964,7 +45986,7 @@
       <c r="F29" s="176"/>
       <c r="G29" s="176"/>
       <c r="H29" s="176"/>
-      <c r="I29" s="188"/>
+      <c r="I29" s="185"/>
       <c r="M29" s="75">
         <v>6.9444444444444397E-3</v>
       </c>
@@ -46231,15 +46253,15 @@
       <c r="I39" s="117"/>
     </row>
     <row r="40" spans="3:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="185" t="s">
+      <c r="C40" s="182" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="186"/>
-      <c r="E40" s="186"/>
-      <c r="F40" s="186"/>
-      <c r="G40" s="186"/>
-      <c r="H40" s="186"/>
-      <c r="I40" s="187"/>
+      <c r="D40" s="183"/>
+      <c r="E40" s="183"/>
+      <c r="F40" s="183"/>
+      <c r="G40" s="183"/>
+      <c r="H40" s="183"/>
+      <c r="I40" s="184"/>
     </row>
     <row r="41" spans="3:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C41" s="97" t="s">
@@ -46336,11 +46358,6 @@
     <row r="45" spans="3:9" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C18:I18"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C40:I40"/>
-    <mergeCell ref="M7:N7"/>
     <mergeCell ref="AB7:AC7"/>
     <mergeCell ref="M6:T6"/>
     <mergeCell ref="V6:AC6"/>
@@ -46348,6 +46365,11 @@
     <mergeCell ref="S7:T7"/>
     <mergeCell ref="V7:W7"/>
     <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C18:I18"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C40:I40"/>
+    <mergeCell ref="M7:N7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -46602,7 +46624,7 @@
       <c r="BT3" s="134"/>
     </row>
     <row r="4" spans="2:88" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="182"/>
+      <c r="B4" s="186"/>
       <c r="C4" s="194"/>
       <c r="D4" s="194"/>
       <c r="E4" s="194"/>
@@ -46620,9 +46642,9 @@
       <c r="Q4" s="194"/>
       <c r="R4" s="194"/>
       <c r="S4" s="194"/>
-      <c r="T4" s="183"/>
+      <c r="T4" s="187"/>
       <c r="U4" s="133"/>
-      <c r="V4" s="182"/>
+      <c r="V4" s="186"/>
       <c r="W4" s="194"/>
       <c r="X4" s="194"/>
       <c r="Y4" s="194"/>
@@ -46640,9 +46662,9 @@
       <c r="AK4" s="194"/>
       <c r="AL4" s="194"/>
       <c r="AM4" s="194"/>
-      <c r="AN4" s="183"/>
+      <c r="AN4" s="187"/>
       <c r="AO4" s="134"/>
-      <c r="AP4" s="182"/>
+      <c r="AP4" s="186"/>
       <c r="AQ4" s="194"/>
       <c r="AR4" s="194"/>
       <c r="AS4" s="194"/>
@@ -46660,7 +46682,7 @@
       <c r="BE4" s="194"/>
       <c r="BF4" s="194"/>
       <c r="BG4" s="194"/>
-      <c r="BH4" s="183"/>
+      <c r="BH4" s="187"/>
       <c r="BI4" s="134"/>
       <c r="BJ4" s="134"/>
       <c r="BK4" s="134"/>
@@ -59581,21 +59603,21 @@
       <c r="CG83" s="135"/>
     </row>
     <row r="84" spans="2:88" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="182"/>
+      <c r="B84" s="186"/>
       <c r="C84" s="194"/>
       <c r="D84" s="194"/>
       <c r="E84" s="194"/>
-      <c r="F84" s="183"/>
-      <c r="H84" s="182"/>
+      <c r="F84" s="187"/>
+      <c r="H84" s="186"/>
       <c r="I84" s="194"/>
       <c r="J84" s="194"/>
       <c r="K84" s="194"/>
-      <c r="L84" s="183"/>
-      <c r="N84" s="182"/>
+      <c r="L84" s="187"/>
+      <c r="N84" s="186"/>
       <c r="O84" s="194"/>
       <c r="P84" s="194"/>
       <c r="Q84" s="194"/>
-      <c r="R84" s="183"/>
+      <c r="R84" s="187"/>
       <c r="T84" s="80"/>
       <c r="U84" s="80"/>
       <c r="AH84" s="132"/>
@@ -67184,7 +67206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91155465-0821-354B-A803-746CB83E7063}">
   <dimension ref="B3:I147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -68082,4 +68104,160 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{366567EE-2038-0845-9A44-27E88E9E6E15}">
+  <dimension ref="C1:K7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="204" t="s">
+        <v>832</v>
+      </c>
+      <c r="E2" s="204"/>
+      <c r="F2" s="204"/>
+      <c r="G2" s="204" t="s">
+        <v>834</v>
+      </c>
+      <c r="H2" s="204"/>
+      <c r="I2" s="204"/>
+      <c r="J2" s="198"/>
+      <c r="K2" s="198"/>
+    </row>
+    <row r="3" spans="3:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="198">
+        <v>7000</v>
+      </c>
+      <c r="E3" s="198">
+        <v>7001</v>
+      </c>
+      <c r="F3" s="198">
+        <v>7002</v>
+      </c>
+      <c r="G3" s="198">
+        <v>7003</v>
+      </c>
+      <c r="H3" s="198">
+        <v>7004</v>
+      </c>
+      <c r="I3" s="198">
+        <v>7005</v>
+      </c>
+      <c r="J3" s="198" t="s">
+        <v>833</v>
+      </c>
+      <c r="K3" s="198" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="198" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="32">
+        <v>1.004618</v>
+      </c>
+      <c r="E4" s="199">
+        <v>1.0296920000000001</v>
+      </c>
+      <c r="F4" s="199">
+        <v>1.016632</v>
+      </c>
+      <c r="G4" s="199">
+        <v>1.0100279999999999</v>
+      </c>
+      <c r="H4" s="199">
+        <v>1.01498</v>
+      </c>
+      <c r="I4" s="199">
+        <v>1.0060359999999999</v>
+      </c>
+      <c r="J4" s="199">
+        <f>SUM(D4:F4)</f>
+        <v>3.050942</v>
+      </c>
+      <c r="K4" s="33">
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="198" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="200">
+        <v>0.92722700000000002</v>
+      </c>
+      <c r="E5" s="201">
+        <v>0.93923100000000004</v>
+      </c>
+      <c r="F5" s="201">
+        <v>0.93503700000000001</v>
+      </c>
+      <c r="G5" s="201">
+        <v>0.93920199999999998</v>
+      </c>
+      <c r="H5" s="201">
+        <v>0.93542400000000003</v>
+      </c>
+      <c r="I5" s="201">
+        <v>0.92906999999999995</v>
+      </c>
+      <c r="J5" s="201">
+        <f t="shared" ref="J5:J6" si="0">SUM(D5:F5)</f>
+        <v>2.8014950000000001</v>
+      </c>
+      <c r="K5" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="198" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="202">
+        <v>2.719738</v>
+      </c>
+      <c r="E6" s="203">
+        <v>2.6514899999999999</v>
+      </c>
+      <c r="F6" s="203">
+        <v>2.676488</v>
+      </c>
+      <c r="G6" s="203">
+        <v>2.6573000000000002</v>
+      </c>
+      <c r="H6" s="203">
+        <v>2.743134</v>
+      </c>
+      <c r="I6" s="203">
+        <v>2.6507299999999998</v>
+      </c>
+      <c r="J6" s="203">
+        <f t="shared" si="0"/>
+        <v>8.0477160000000012</v>
+      </c>
+      <c r="K6" s="35">
+        <v>6.49</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>